<commit_message>
Convert report from html to word document. Add AIC, BIC, and chi-square model comparison results to final table in manuscript. Close issue #5.
</commit_message>
<xml_diff>
--- a/cumulative_results.xlsx
+++ b/cumulative_results.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I118"/>
+  <dimension ref="A1:Q118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -403,6 +403,46 @@
           <t>upper</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>npar</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>AIC</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>BIC</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>logLik</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>deviance</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Chisq</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Df</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Pr(&gt;Chisq)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -431,10 +471,25 @@
         <v>0.04964264048460895</v>
       </c>
       <c r="H2">
-        <v>0.3069209018816848</v>
+        <v>0.2862340954906926</v>
       </c>
       <c r="I2">
-        <v>1.741727816232951</v>
+        <v>1.648967338964327</v>
+      </c>
+      <c r="J2">
+        <v>16</v>
+      </c>
+      <c r="K2">
+        <v>1312.56295726069</v>
+      </c>
+      <c r="L2">
+        <v>1373.396851266723</v>
+      </c>
+      <c r="M2">
+        <v>-640.2814786303452</v>
+      </c>
+      <c r="N2">
+        <v>1280.56295726069</v>
       </c>
     </row>
     <row r="3">
@@ -464,10 +519,25 @@
         <v>0.6028693164558701</v>
       </c>
       <c r="H3">
-        <v>-0.5331820768566752</v>
+        <v>-0.3856633561857863</v>
       </c>
       <c r="I3">
-        <v>0.759499803023241</v>
+        <v>0.7109394422838996</v>
+      </c>
+      <c r="J3">
+        <v>16</v>
+      </c>
+      <c r="K3">
+        <v>1312.56295726069</v>
+      </c>
+      <c r="L3">
+        <v>1373.396851266723</v>
+      </c>
+      <c r="M3">
+        <v>-640.2814786303452</v>
+      </c>
+      <c r="N3">
+        <v>1280.56295726069</v>
       </c>
     </row>
     <row r="4">
@@ -497,10 +567,25 @@
         <v>0.386240323001902</v>
       </c>
       <c r="H4">
-        <v>-0.7737002888103131</v>
+        <v>-0.75872991513925</v>
       </c>
       <c r="I4">
-        <v>0.3144149942926784</v>
+        <v>0.2683497172284998</v>
+      </c>
+      <c r="J4">
+        <v>16</v>
+      </c>
+      <c r="K4">
+        <v>1312.56295726069</v>
+      </c>
+      <c r="L4">
+        <v>1373.396851266723</v>
+      </c>
+      <c r="M4">
+        <v>-640.2814786303452</v>
+      </c>
+      <c r="N4">
+        <v>1280.56295726069</v>
       </c>
     </row>
     <row r="5">
@@ -530,10 +615,25 @@
         <v>0.03659352146781997</v>
       </c>
       <c r="H5">
-        <v>-1.047970796498991</v>
+        <v>-1.01890985232992</v>
       </c>
       <c r="I5">
-        <v>-0.02166874387469865</v>
+        <v>0.04640187659852996</v>
+      </c>
+      <c r="J5">
+        <v>16</v>
+      </c>
+      <c r="K5">
+        <v>1312.56295726069</v>
+      </c>
+      <c r="L5">
+        <v>1373.396851266723</v>
+      </c>
+      <c r="M5">
+        <v>-640.2814786303452</v>
+      </c>
+      <c r="N5">
+        <v>1280.56295726069</v>
       </c>
     </row>
     <row r="6">
@@ -563,10 +663,25 @@
         <v>0.02865195558438659</v>
       </c>
       <c r="H6">
-        <v>0.0262788860644401</v>
+        <v>0.006562047272790326</v>
       </c>
       <c r="I6">
-        <v>0.4571100061287585</v>
+        <v>0.4529963286423255</v>
+      </c>
+      <c r="J6">
+        <v>16</v>
+      </c>
+      <c r="K6">
+        <v>1312.56295726069</v>
+      </c>
+      <c r="L6">
+        <v>1373.396851266723</v>
+      </c>
+      <c r="M6">
+        <v>-640.2814786303452</v>
+      </c>
+      <c r="N6">
+        <v>1280.56295726069</v>
       </c>
     </row>
     <row r="7">
@@ -596,10 +711,25 @@
         <v>0.9448898796854626</v>
       </c>
       <c r="H7">
-        <v>-0.1979151506112642</v>
+        <v>-0.209186906951652</v>
       </c>
       <c r="I7">
-        <v>0.2178628615917741</v>
+        <v>0.216223496922463</v>
+      </c>
+      <c r="J7">
+        <v>16</v>
+      </c>
+      <c r="K7">
+        <v>1312.56295726069</v>
+      </c>
+      <c r="L7">
+        <v>1373.396851266723</v>
+      </c>
+      <c r="M7">
+        <v>-640.2814786303452</v>
+      </c>
+      <c r="N7">
+        <v>1280.56295726069</v>
       </c>
     </row>
     <row r="8">
@@ -629,10 +759,25 @@
         <v>0.2932670504991191</v>
       </c>
       <c r="H8">
-        <v>-0.5685731351198786</v>
+        <v>-0.5420026229208045</v>
       </c>
       <c r="I8">
-        <v>0.1490249654206023</v>
+        <v>0.2049381797783333</v>
+      </c>
+      <c r="J8">
+        <v>16</v>
+      </c>
+      <c r="K8">
+        <v>1312.56295726069</v>
+      </c>
+      <c r="L8">
+        <v>1373.396851266723</v>
+      </c>
+      <c r="M8">
+        <v>-640.2814786303452</v>
+      </c>
+      <c r="N8">
+        <v>1280.56295726069</v>
       </c>
     </row>
     <row r="9">
@@ -662,10 +807,25 @@
         <v>0.07750829082893188</v>
       </c>
       <c r="H9">
-        <v>-0.5715970610093958</v>
+        <v>-0.594090219936199</v>
       </c>
       <c r="I9">
-        <v>0.06350303243048017</v>
+        <v>0.06775443910799996</v>
+      </c>
+      <c r="J9">
+        <v>16</v>
+      </c>
+      <c r="K9">
+        <v>1312.56295726069</v>
+      </c>
+      <c r="L9">
+        <v>1373.396851266723</v>
+      </c>
+      <c r="M9">
+        <v>-640.2814786303452</v>
+      </c>
+      <c r="N9">
+        <v>1280.56295726069</v>
       </c>
     </row>
     <row r="10">
@@ -695,10 +855,25 @@
         <v>0.817717335487248</v>
       </c>
       <c r="H10">
-        <v>-0.2255790400718585</v>
+        <v>-0.2078895971868763</v>
       </c>
       <c r="I10">
-        <v>0.2464239887215125</v>
+        <v>0.2758790143920343</v>
+      </c>
+      <c r="J10">
+        <v>16</v>
+      </c>
+      <c r="K10">
+        <v>1312.56295726069</v>
+      </c>
+      <c r="L10">
+        <v>1373.396851266723</v>
+      </c>
+      <c r="M10">
+        <v>-640.2814786303452</v>
+      </c>
+      <c r="N10">
+        <v>1280.56295726069</v>
       </c>
     </row>
     <row r="11">
@@ -728,10 +903,25 @@
         <v>0.5634618251164623</v>
       </c>
       <c r="H11">
-        <v>-0.3434214135987804</v>
+        <v>-0.3303061346749652</v>
       </c>
       <c r="I11">
-        <v>0.1685775450593807</v>
+        <v>0.1685190126524619</v>
+      </c>
+      <c r="J11">
+        <v>16</v>
+      </c>
+      <c r="K11">
+        <v>1312.56295726069</v>
+      </c>
+      <c r="L11">
+        <v>1373.396851266723</v>
+      </c>
+      <c r="M11">
+        <v>-640.2814786303452</v>
+      </c>
+      <c r="N11">
+        <v>1280.56295726069</v>
       </c>
     </row>
     <row r="12">
@@ -761,10 +951,25 @@
         <v>0.2400809627951311</v>
       </c>
       <c r="H12">
-        <v>-0.1827219819357007</v>
+        <v>-0.185218066585658</v>
       </c>
       <c r="I12">
-        <v>0.7526125487991261</v>
+        <v>0.7447657300540489</v>
+      </c>
+      <c r="J12">
+        <v>16</v>
+      </c>
+      <c r="K12">
+        <v>1312.56295726069</v>
+      </c>
+      <c r="L12">
+        <v>1373.396851266723</v>
+      </c>
+      <c r="M12">
+        <v>-640.2814786303452</v>
+      </c>
+      <c r="N12">
+        <v>1280.56295726069</v>
       </c>
     </row>
     <row r="13">
@@ -794,10 +999,25 @@
         <v>0.3064575649738183</v>
       </c>
       <c r="H13">
-        <v>-0.2431266289084113</v>
+        <v>-0.2038332389873086</v>
       </c>
       <c r="I13">
-        <v>0.6544090653082518</v>
+        <v>0.7191129042648454</v>
+      </c>
+      <c r="J13">
+        <v>16</v>
+      </c>
+      <c r="K13">
+        <v>1312.56295726069</v>
+      </c>
+      <c r="L13">
+        <v>1373.396851266723</v>
+      </c>
+      <c r="M13">
+        <v>-640.2814786303452</v>
+      </c>
+      <c r="N13">
+        <v>1280.56295726069</v>
       </c>
     </row>
     <row r="14">
@@ -827,10 +1047,25 @@
         <v>0.6054857849294826</v>
       </c>
       <c r="H14">
-        <v>-0.4702450616975595</v>
+        <v>-0.4549225709284624</v>
       </c>
       <c r="I14">
-        <v>0.2178830804406787</v>
+        <v>0.2208791779373557</v>
+      </c>
+      <c r="J14">
+        <v>16</v>
+      </c>
+      <c r="K14">
+        <v>1312.56295726069</v>
+      </c>
+      <c r="L14">
+        <v>1373.396851266723</v>
+      </c>
+      <c r="M14">
+        <v>-640.2814786303452</v>
+      </c>
+      <c r="N14">
+        <v>1280.56295726069</v>
       </c>
     </row>
     <row r="15">
@@ -860,10 +1095,34 @@
         <v>0.05812185553694306</v>
       </c>
       <c r="H15">
-        <v>0.251956429958556</v>
+        <v>0.3503323524768479</v>
       </c>
       <c r="I15">
-        <v>1.72851500534969</v>
+        <v>1.678295774196313</v>
+      </c>
+      <c r="J15">
+        <v>18</v>
+      </c>
+      <c r="K15">
+        <v>1305.807720409842</v>
+      </c>
+      <c r="L15">
+        <v>1374.24585116663</v>
+      </c>
+      <c r="M15">
+        <v>-634.9038602049212</v>
+      </c>
+      <c r="N15">
+        <v>1269.807720409842</v>
+      </c>
+      <c r="O15">
+        <v>10.75523685084795</v>
+      </c>
+      <c r="P15">
+        <v>2</v>
+      </c>
+      <c r="Q15">
+        <v>0.004618808879478783</v>
       </c>
     </row>
     <row r="16">
@@ -893,10 +1152,34 @@
         <v>0.004307415602908025</v>
       </c>
       <c r="H16">
-        <v>0.3366010018743768</v>
+        <v>0.2954894333941566</v>
       </c>
       <c r="I16">
-        <v>1.771729374873538</v>
+        <v>1.85059744763241</v>
+      </c>
+      <c r="J16">
+        <v>18</v>
+      </c>
+      <c r="K16">
+        <v>1305.807720409842</v>
+      </c>
+      <c r="L16">
+        <v>1374.24585116663</v>
+      </c>
+      <c r="M16">
+        <v>-634.9038602049212</v>
+      </c>
+      <c r="N16">
+        <v>1269.807720409842</v>
+      </c>
+      <c r="O16">
+        <v>10.75523685084795</v>
+      </c>
+      <c r="P16">
+        <v>2</v>
+      </c>
+      <c r="Q16">
+        <v>0.004618808879478783</v>
       </c>
     </row>
     <row r="17">
@@ -926,10 +1209,34 @@
         <v>0.5155238728790634</v>
       </c>
       <c r="H17">
-        <v>-0.8490241269438108</v>
+        <v>-0.7993290502379676</v>
       </c>
       <c r="I17">
-        <v>0.3719848506098375</v>
+        <v>0.3574556335416999</v>
+      </c>
+      <c r="J17">
+        <v>18</v>
+      </c>
+      <c r="K17">
+        <v>1305.807720409842</v>
+      </c>
+      <c r="L17">
+        <v>1374.24585116663</v>
+      </c>
+      <c r="M17">
+        <v>-634.9038602049212</v>
+      </c>
+      <c r="N17">
+        <v>1269.807720409842</v>
+      </c>
+      <c r="O17">
+        <v>10.75523685084795</v>
+      </c>
+      <c r="P17">
+        <v>2</v>
+      </c>
+      <c r="Q17">
+        <v>0.004618808879478783</v>
       </c>
     </row>
     <row r="18">
@@ -959,10 +1266,34 @@
         <v>0.678039927149849</v>
       </c>
       <c r="H18">
-        <v>-0.6802391574970994</v>
+        <v>-0.65716948170628</v>
       </c>
       <c r="I18">
-        <v>0.3912384891832481</v>
+        <v>0.4342156524684461</v>
+      </c>
+      <c r="J18">
+        <v>18</v>
+      </c>
+      <c r="K18">
+        <v>1305.807720409842</v>
+      </c>
+      <c r="L18">
+        <v>1374.24585116663</v>
+      </c>
+      <c r="M18">
+        <v>-634.9038602049212</v>
+      </c>
+      <c r="N18">
+        <v>1269.807720409842</v>
+      </c>
+      <c r="O18">
+        <v>10.75523685084795</v>
+      </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>0.004618808879478783</v>
       </c>
     </row>
     <row r="19">
@@ -992,10 +1323,34 @@
         <v>0.4090643909381595</v>
       </c>
       <c r="H19">
-        <v>-0.8503546404329602</v>
+        <v>-0.8610621813422327</v>
       </c>
       <c r="I19">
-        <v>0.295771635079566</v>
+        <v>0.3128270876381522</v>
+      </c>
+      <c r="J19">
+        <v>18</v>
+      </c>
+      <c r="K19">
+        <v>1305.807720409842</v>
+      </c>
+      <c r="L19">
+        <v>1374.24585116663</v>
+      </c>
+      <c r="M19">
+        <v>-634.9038602049212</v>
+      </c>
+      <c r="N19">
+        <v>1269.807720409842</v>
+      </c>
+      <c r="O19">
+        <v>10.75523685084795</v>
+      </c>
+      <c r="P19">
+        <v>2</v>
+      </c>
+      <c r="Q19">
+        <v>0.004618808879478783</v>
       </c>
     </row>
     <row r="20">
@@ -1025,10 +1380,34 @@
         <v>0.03279137701991269</v>
       </c>
       <c r="H20">
-        <v>-1.629699222923398</v>
+        <v>-1.584011153275394</v>
       </c>
       <c r="I20">
-        <v>-0.1515334313904968</v>
+        <v>-0.03264317216036437</v>
+      </c>
+      <c r="J20">
+        <v>18</v>
+      </c>
+      <c r="K20">
+        <v>1305.807720409842</v>
+      </c>
+      <c r="L20">
+        <v>1374.24585116663</v>
+      </c>
+      <c r="M20">
+        <v>-634.9038602049212</v>
+      </c>
+      <c r="N20">
+        <v>1269.807720409842</v>
+      </c>
+      <c r="O20">
+        <v>10.75523685084795</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <v>0.004618808879478783</v>
       </c>
     </row>
     <row r="21">
@@ -1058,10 +1437,34 @@
         <v>0.02760057400643724</v>
       </c>
       <c r="H21">
-        <v>0.001855405571353184</v>
+        <v>0.02458238190772083</v>
       </c>
       <c r="I21">
-        <v>0.4551650302055547</v>
+        <v>0.4529090083278975</v>
+      </c>
+      <c r="J21">
+        <v>18</v>
+      </c>
+      <c r="K21">
+        <v>1305.807720409842</v>
+      </c>
+      <c r="L21">
+        <v>1374.24585116663</v>
+      </c>
+      <c r="M21">
+        <v>-634.9038602049212</v>
+      </c>
+      <c r="N21">
+        <v>1269.807720409842</v>
+      </c>
+      <c r="O21">
+        <v>10.75523685084795</v>
+      </c>
+      <c r="P21">
+        <v>2</v>
+      </c>
+      <c r="Q21">
+        <v>0.004618808879478783</v>
       </c>
     </row>
     <row r="22">
@@ -1091,10 +1494,34 @@
         <v>0.6799018601661131</v>
       </c>
       <c r="H22">
-        <v>-0.1642742329324593</v>
+        <v>-0.1604459511345854</v>
       </c>
       <c r="I22">
-        <v>0.2742036269060251</v>
+        <v>0.2454738191131656</v>
+      </c>
+      <c r="J22">
+        <v>18</v>
+      </c>
+      <c r="K22">
+        <v>1305.807720409842</v>
+      </c>
+      <c r="L22">
+        <v>1374.24585116663</v>
+      </c>
+      <c r="M22">
+        <v>-634.9038602049212</v>
+      </c>
+      <c r="N22">
+        <v>1269.807720409842</v>
+      </c>
+      <c r="O22">
+        <v>10.75523685084795</v>
+      </c>
+      <c r="P22">
+        <v>2</v>
+      </c>
+      <c r="Q22">
+        <v>0.004618808879478783</v>
       </c>
     </row>
     <row r="23">
@@ -1124,10 +1551,34 @@
         <v>0.3882036853072163</v>
       </c>
       <c r="H23">
-        <v>-0.506042227720426</v>
+        <v>-0.4762321292867966</v>
       </c>
       <c r="I23">
-        <v>0.226750644132869</v>
+        <v>0.2121530345600002</v>
+      </c>
+      <c r="J23">
+        <v>18</v>
+      </c>
+      <c r="K23">
+        <v>1305.807720409842</v>
+      </c>
+      <c r="L23">
+        <v>1374.24585116663</v>
+      </c>
+      <c r="M23">
+        <v>-634.9038602049212</v>
+      </c>
+      <c r="N23">
+        <v>1269.807720409842</v>
+      </c>
+      <c r="O23">
+        <v>10.75523685084795</v>
+      </c>
+      <c r="P23">
+        <v>2</v>
+      </c>
+      <c r="Q23">
+        <v>0.004618808879478783</v>
       </c>
     </row>
     <row r="24">
@@ -1157,10 +1608,34 @@
         <v>0.1670040167557344</v>
       </c>
       <c r="H24">
-        <v>-0.5383929634374526</v>
+        <v>-0.5390743257483683</v>
       </c>
       <c r="I24">
-        <v>0.07757246495268476</v>
+        <v>0.08497938811892621</v>
+      </c>
+      <c r="J24">
+        <v>18</v>
+      </c>
+      <c r="K24">
+        <v>1305.807720409842</v>
+      </c>
+      <c r="L24">
+        <v>1374.24585116663</v>
+      </c>
+      <c r="M24">
+        <v>-634.9038602049212</v>
+      </c>
+      <c r="N24">
+        <v>1269.807720409842</v>
+      </c>
+      <c r="O24">
+        <v>10.75523685084795</v>
+      </c>
+      <c r="P24">
+        <v>2</v>
+      </c>
+      <c r="Q24">
+        <v>0.004618808879478783</v>
       </c>
     </row>
     <row r="25">
@@ -1190,10 +1665,34 @@
         <v>0.9928509467147366</v>
       </c>
       <c r="H25">
-        <v>-0.2312174946874582</v>
+        <v>-0.2215532296616132</v>
       </c>
       <c r="I25">
-        <v>0.245712308144347</v>
+        <v>0.2444659215465013</v>
+      </c>
+      <c r="J25">
+        <v>18</v>
+      </c>
+      <c r="K25">
+        <v>1305.807720409842</v>
+      </c>
+      <c r="L25">
+        <v>1374.24585116663</v>
+      </c>
+      <c r="M25">
+        <v>-634.9038602049212</v>
+      </c>
+      <c r="N25">
+        <v>1269.807720409842</v>
+      </c>
+      <c r="O25">
+        <v>10.75523685084795</v>
+      </c>
+      <c r="P25">
+        <v>2</v>
+      </c>
+      <c r="Q25">
+        <v>0.004618808879478783</v>
       </c>
     </row>
     <row r="26">
@@ -1223,10 +1722,34 @@
         <v>0.789229887055815</v>
       </c>
       <c r="H26">
-        <v>-0.285776959456242</v>
+        <v>-0.2844730655598888</v>
       </c>
       <c r="I26">
-        <v>0.2110009589875045</v>
+        <v>0.198991600251633</v>
+      </c>
+      <c r="J26">
+        <v>18</v>
+      </c>
+      <c r="K26">
+        <v>1305.807720409842</v>
+      </c>
+      <c r="L26">
+        <v>1374.24585116663</v>
+      </c>
+      <c r="M26">
+        <v>-634.9038602049212</v>
+      </c>
+      <c r="N26">
+        <v>1269.807720409842</v>
+      </c>
+      <c r="O26">
+        <v>10.75523685084795</v>
+      </c>
+      <c r="P26">
+        <v>2</v>
+      </c>
+      <c r="Q26">
+        <v>0.004618808879478783</v>
       </c>
     </row>
     <row r="27">
@@ -1256,10 +1779,34 @@
         <v>0.325594064051256</v>
       </c>
       <c r="H27">
-        <v>-0.2457588271564176</v>
+        <v>-0.2821687751094802</v>
       </c>
       <c r="I27">
-        <v>0.6855663649185361</v>
+        <v>0.688194791328801</v>
+      </c>
+      <c r="J27">
+        <v>18</v>
+      </c>
+      <c r="K27">
+        <v>1305.807720409842</v>
+      </c>
+      <c r="L27">
+        <v>1374.24585116663</v>
+      </c>
+      <c r="M27">
+        <v>-634.9038602049212</v>
+      </c>
+      <c r="N27">
+        <v>1269.807720409842</v>
+      </c>
+      <c r="O27">
+        <v>10.75523685084795</v>
+      </c>
+      <c r="P27">
+        <v>2</v>
+      </c>
+      <c r="Q27">
+        <v>0.004618808879478783</v>
       </c>
     </row>
     <row r="28">
@@ -1289,10 +1836,34 @@
         <v>0.4106991278636435</v>
       </c>
       <c r="H28">
-        <v>-0.2290251351152283</v>
+        <v>-0.2407674385682356</v>
       </c>
       <c r="I28">
-        <v>0.6104189567926602</v>
+        <v>0.6128732183646094</v>
+      </c>
+      <c r="J28">
+        <v>18</v>
+      </c>
+      <c r="K28">
+        <v>1305.807720409842</v>
+      </c>
+      <c r="L28">
+        <v>1374.24585116663</v>
+      </c>
+      <c r="M28">
+        <v>-634.9038602049212</v>
+      </c>
+      <c r="N28">
+        <v>1269.807720409842</v>
+      </c>
+      <c r="O28">
+        <v>10.75523685084795</v>
+      </c>
+      <c r="P28">
+        <v>2</v>
+      </c>
+      <c r="Q28">
+        <v>0.004618808879478783</v>
       </c>
     </row>
     <row r="29">
@@ -1322,10 +1893,34 @@
         <v>0.4271125636813243</v>
       </c>
       <c r="H29">
-        <v>-0.493688797991767</v>
+        <v>-0.4625301030330881</v>
       </c>
       <c r="I29">
-        <v>0.2025237809450629</v>
+        <v>0.1911731166775313</v>
+      </c>
+      <c r="J29">
+        <v>18</v>
+      </c>
+      <c r="K29">
+        <v>1305.807720409842</v>
+      </c>
+      <c r="L29">
+        <v>1374.24585116663</v>
+      </c>
+      <c r="M29">
+        <v>-634.9038602049212</v>
+      </c>
+      <c r="N29">
+        <v>1269.807720409842</v>
+      </c>
+      <c r="O29">
+        <v>10.75523685084795</v>
+      </c>
+      <c r="P29">
+        <v>2</v>
+      </c>
+      <c r="Q29">
+        <v>0.004618808879478783</v>
       </c>
     </row>
     <row r="30">
@@ -1355,10 +1950,34 @@
         <v>0.06252292722425552</v>
       </c>
       <c r="H30">
-        <v>0.2101770240576655</v>
+        <v>0.3125829819526447</v>
       </c>
       <c r="I30">
-        <v>1.648281432330497</v>
+        <v>1.609924375241359</v>
+      </c>
+      <c r="J30">
+        <v>19</v>
+      </c>
+      <c r="K30">
+        <v>1308.855755021857</v>
+      </c>
+      <c r="L30">
+        <v>1381.096004154021</v>
+      </c>
+      <c r="M30">
+        <v>-635.4278775109285</v>
+      </c>
+      <c r="N30">
+        <v>1270.855755021857</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -1388,10 +2007,34 @@
         <v>0.004849334745694508</v>
       </c>
       <c r="H31">
-        <v>0.4254027431318351</v>
+        <v>0.33032748846421</v>
       </c>
       <c r="I31">
-        <v>2.209638081207873</v>
+        <v>2.190418517249494</v>
+      </c>
+      <c r="J31">
+        <v>19</v>
+      </c>
+      <c r="K31">
+        <v>1308.855755021857</v>
+      </c>
+      <c r="L31">
+        <v>1381.096004154021</v>
+      </c>
+      <c r="M31">
+        <v>-635.4278775109285</v>
+      </c>
+      <c r="N31">
+        <v>1270.855755021857</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1421,10 +2064,34 @@
         <v>0.9186748126778145</v>
       </c>
       <c r="H32">
-        <v>-0.7220347162306118</v>
+        <v>-0.734644387179208</v>
       </c>
       <c r="I32">
-        <v>0.6219678794868515</v>
+        <v>0.6831429284207239</v>
+      </c>
+      <c r="J32">
+        <v>19</v>
+      </c>
+      <c r="K32">
+        <v>1308.855755021857</v>
+      </c>
+      <c r="L32">
+        <v>1381.096004154021</v>
+      </c>
+      <c r="M32">
+        <v>-635.4278775109285</v>
+      </c>
+      <c r="N32">
+        <v>1270.855755021857</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1454,10 +2121,34 @@
         <v>0.4481234189980438</v>
       </c>
       <c r="H33">
-        <v>-0.7807192929348717</v>
+        <v>-0.7964892139021089</v>
       </c>
       <c r="I33">
-        <v>0.374227983571693</v>
+        <v>0.3066575248178697</v>
+      </c>
+      <c r="J33">
+        <v>19</v>
+      </c>
+      <c r="K33">
+        <v>1308.855755021857</v>
+      </c>
+      <c r="L33">
+        <v>1381.096004154021</v>
+      </c>
+      <c r="M33">
+        <v>-635.4278775109285</v>
+      </c>
+      <c r="N33">
+        <v>1270.855755021857</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1487,10 +2178,34 @@
         <v>0.3671602410124577</v>
       </c>
       <c r="H34">
-        <v>-0.8609852877159415</v>
+        <v>-0.8396189919628324</v>
       </c>
       <c r="I34">
-        <v>0.2972058953064973</v>
+        <v>0.2812554753050258</v>
+      </c>
+      <c r="J34">
+        <v>19</v>
+      </c>
+      <c r="K34">
+        <v>1308.855755021857</v>
+      </c>
+      <c r="L34">
+        <v>1381.096004154021</v>
+      </c>
+      <c r="M34">
+        <v>-635.4278775109285</v>
+      </c>
+      <c r="N34">
+        <v>1270.855755021857</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>1</v>
+      </c>
+      <c r="Q34">
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -1520,10 +2235,34 @@
         <v>0.7668946240781603</v>
       </c>
       <c r="H35">
-        <v>-0.7757245067579137</v>
+        <v>-0.7594545357787538</v>
       </c>
       <c r="I35">
-        <v>0.5631500345808723</v>
+        <v>0.5402843201127598</v>
+      </c>
+      <c r="J35">
+        <v>19</v>
+      </c>
+      <c r="K35">
+        <v>1308.855755021857</v>
+      </c>
+      <c r="L35">
+        <v>1381.096004154021</v>
+      </c>
+      <c r="M35">
+        <v>-635.4278775109285</v>
+      </c>
+      <c r="N35">
+        <v>1270.855755021857</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>1</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1553,10 +2292,34 @@
         <v>0.03108283570422055</v>
       </c>
       <c r="H36">
-        <v>-1.891762520054973</v>
+        <v>-1.738115458740259</v>
       </c>
       <c r="I36">
-        <v>-0.1166646954134128</v>
+        <v>-0.04179908567843431</v>
+      </c>
+      <c r="J36">
+        <v>19</v>
+      </c>
+      <c r="K36">
+        <v>1308.855755021857</v>
+      </c>
+      <c r="L36">
+        <v>1381.096004154021</v>
+      </c>
+      <c r="M36">
+        <v>-635.4278775109285</v>
+      </c>
+      <c r="N36">
+        <v>1270.855755021857</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>1</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1586,10 +2349,34 @@
         <v>0.02175506015455142</v>
       </c>
       <c r="H37">
-        <v>0.06330029031348122</v>
+        <v>0.01115372992588829</v>
       </c>
       <c r="I37">
-        <v>0.4794748024910525</v>
+        <v>0.4533302956142493</v>
+      </c>
+      <c r="J37">
+        <v>19</v>
+      </c>
+      <c r="K37">
+        <v>1308.855755021857</v>
+      </c>
+      <c r="L37">
+        <v>1381.096004154021</v>
+      </c>
+      <c r="M37">
+        <v>-635.4278775109285</v>
+      </c>
+      <c r="N37">
+        <v>1270.855755021857</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>1</v>
+      </c>
+      <c r="Q37">
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1619,10 +2406,34 @@
         <v>0.6977696725009876</v>
       </c>
       <c r="H38">
-        <v>-0.1926972394255149</v>
+        <v>-0.1712367182825224</v>
       </c>
       <c r="I38">
-        <v>0.2312856259888359</v>
+        <v>0.2455096365025987</v>
+      </c>
+      <c r="J38">
+        <v>19</v>
+      </c>
+      <c r="K38">
+        <v>1308.855755021857</v>
+      </c>
+      <c r="L38">
+        <v>1381.096004154021</v>
+      </c>
+      <c r="M38">
+        <v>-635.4278775109285</v>
+      </c>
+      <c r="N38">
+        <v>1270.855755021857</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>1</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1652,10 +2463,34 @@
         <v>0.3802621071032635</v>
       </c>
       <c r="H39">
-        <v>-0.5651330074247481</v>
+        <v>-0.5002049795210112</v>
       </c>
       <c r="I39">
-        <v>0.2158296829276786</v>
+        <v>0.191529337971982</v>
+      </c>
+      <c r="J39">
+        <v>19</v>
+      </c>
+      <c r="K39">
+        <v>1308.855755021857</v>
+      </c>
+      <c r="L39">
+        <v>1381.096004154021</v>
+      </c>
+      <c r="M39">
+        <v>-635.4278775109285</v>
+      </c>
+      <c r="N39">
+        <v>1270.855755021857</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>1</v>
+      </c>
+      <c r="Q39">
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -1685,10 +2520,34 @@
         <v>0.1410514875989229</v>
       </c>
       <c r="H40">
-        <v>-0.5505982074884667</v>
+        <v>-0.5455031111243596</v>
       </c>
       <c r="I40">
-        <v>0.08830397579955485</v>
+        <v>0.07736329385446518</v>
+      </c>
+      <c r="J40">
+        <v>19</v>
+      </c>
+      <c r="K40">
+        <v>1308.855755021857</v>
+      </c>
+      <c r="L40">
+        <v>1381.096004154021</v>
+      </c>
+      <c r="M40">
+        <v>-635.4278775109285</v>
+      </c>
+      <c r="N40">
+        <v>1270.855755021857</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>1</v>
+      </c>
+      <c r="Q40">
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -1718,10 +2577,34 @@
         <v>0.8959805637514762</v>
       </c>
       <c r="H41">
-        <v>-0.2081853161064861</v>
+        <v>-0.2028372948973302</v>
       </c>
       <c r="I41">
-        <v>0.2551802887857036</v>
+        <v>0.2493083657628704</v>
+      </c>
+      <c r="J41">
+        <v>19</v>
+      </c>
+      <c r="K41">
+        <v>1308.855755021857</v>
+      </c>
+      <c r="L41">
+        <v>1381.096004154021</v>
+      </c>
+      <c r="M41">
+        <v>-635.4278775109285</v>
+      </c>
+      <c r="N41">
+        <v>1270.855755021857</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>1</v>
+      </c>
+      <c r="Q41">
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1751,10 +2634,34 @@
         <v>0.68815076450387</v>
       </c>
       <c r="H42">
-        <v>-0.3160568998587638</v>
+        <v>-0.3218395372746429</v>
       </c>
       <c r="I42">
-        <v>0.2237311093425588</v>
+        <v>0.2074403738074544</v>
+      </c>
+      <c r="J42">
+        <v>19</v>
+      </c>
+      <c r="K42">
+        <v>1308.855755021857</v>
+      </c>
+      <c r="L42">
+        <v>1381.096004154021</v>
+      </c>
+      <c r="M42">
+        <v>-635.4278775109285</v>
+      </c>
+      <c r="N42">
+        <v>1270.855755021857</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>1</v>
+      </c>
+      <c r="Q42">
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -1784,10 +2691,34 @@
         <v>0.2290822980262702</v>
       </c>
       <c r="H43">
-        <v>-0.2190830682540639</v>
+        <v>-0.1985776008259142</v>
       </c>
       <c r="I43">
-        <v>0.7920900465664917</v>
+        <v>0.765280334170213</v>
+      </c>
+      <c r="J43">
+        <v>19</v>
+      </c>
+      <c r="K43">
+        <v>1308.855755021857</v>
+      </c>
+      <c r="L43">
+        <v>1381.096004154021</v>
+      </c>
+      <c r="M43">
+        <v>-635.4278775109285</v>
+      </c>
+      <c r="N43">
+        <v>1270.855755021857</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>1</v>
+      </c>
+      <c r="Q43">
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -1817,10 +2748,34 @@
         <v>0.2501239398540214</v>
       </c>
       <c r="H44">
-        <v>-0.1616901466226421</v>
+        <v>-0.1785622044193332</v>
       </c>
       <c r="I44">
-        <v>0.7207162179874436</v>
+        <v>0.7211604152695491</v>
+      </c>
+      <c r="J44">
+        <v>19</v>
+      </c>
+      <c r="K44">
+        <v>1308.855755021857</v>
+      </c>
+      <c r="L44">
+        <v>1381.096004154021</v>
+      </c>
+      <c r="M44">
+        <v>-635.4278775109285</v>
+      </c>
+      <c r="N44">
+        <v>1270.855755021857</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>1</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -1850,10 +2805,34 @@
         <v>0.4913382811027023</v>
       </c>
       <c r="H45">
-        <v>-0.4424510506062306</v>
+        <v>-0.4165754255433853</v>
       </c>
       <c r="I45">
-        <v>0.1940853522884545</v>
+        <v>0.2152630253709437</v>
+      </c>
+      <c r="J45">
+        <v>19</v>
+      </c>
+      <c r="K45">
+        <v>1308.855755021857</v>
+      </c>
+      <c r="L45">
+        <v>1381.096004154021</v>
+      </c>
+      <c r="M45">
+        <v>-635.4278775109285</v>
+      </c>
+      <c r="N45">
+        <v>1270.855755021857</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>1</v>
+      </c>
+      <c r="Q45">
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -1883,10 +2862,10 @@
         <v>0.06297009607337689</v>
       </c>
       <c r="H46">
-        <v>0.1831327346264899</v>
+        <v>0.155808429375246</v>
       </c>
       <c r="I46">
-        <v>1.622159316542892</v>
+        <v>1.622986304153297</v>
       </c>
     </row>
     <row r="47">
@@ -1916,10 +2895,10 @@
         <v>0.005049185733957656</v>
       </c>
       <c r="H47">
-        <v>0.4153619068645605</v>
+        <v>0.4079785539316004</v>
       </c>
       <c r="I47">
-        <v>2.047115088401197</v>
+        <v>2.027418079898665</v>
       </c>
     </row>
     <row r="48">
@@ -1949,10 +2928,10 @@
         <v>0.8637447796552011</v>
       </c>
       <c r="H48">
-        <v>-0.8321207088959371</v>
+        <v>-0.7665783931071387</v>
       </c>
       <c r="I48">
-        <v>0.7833954371098191</v>
+        <v>0.6853448030848063</v>
       </c>
     </row>
     <row r="49">
@@ -1982,10 +2961,10 @@
         <v>0.7142314729337769</v>
       </c>
       <c r="H49">
-        <v>-0.4979592984137305</v>
+        <v>-0.6142831104819919</v>
       </c>
       <c r="I49">
-        <v>0.7328082249678616</v>
+        <v>0.7710330737280957</v>
       </c>
     </row>
     <row r="50">
@@ -2015,10 +2994,10 @@
         <v>0.409779029170831</v>
       </c>
       <c r="H50">
-        <v>-0.8024758438480389</v>
+        <v>-0.7507291499353248</v>
       </c>
       <c r="I50">
-        <v>0.3434005588401803</v>
+        <v>0.3442006450209224</v>
       </c>
     </row>
     <row r="51">
@@ -2048,10 +3027,10 @@
         <v>0.5970401227461903</v>
       </c>
       <c r="H51">
-        <v>-0.853752653517689</v>
+        <v>-0.8687266060483141</v>
       </c>
       <c r="I51">
-        <v>0.4980674372987422</v>
+        <v>0.5070316976568988</v>
       </c>
     </row>
     <row r="52">
@@ -2081,10 +3060,10 @@
         <v>0.2563739878656627</v>
       </c>
       <c r="H52">
-        <v>-1.13440621879657</v>
+        <v>-1.103917488190971</v>
       </c>
       <c r="I52">
-        <v>0.218061949738156</v>
+        <v>0.3163342809448065</v>
       </c>
     </row>
     <row r="53">
@@ -2114,10 +3093,10 @@
         <v>0.1452463571798465</v>
       </c>
       <c r="H53">
-        <v>-1.777909831762065</v>
+        <v>-1.721754345843732</v>
       </c>
       <c r="I53">
-        <v>0.2918691548078446</v>
+        <v>0.264307641549676</v>
       </c>
     </row>
     <row r="54">
@@ -2147,10 +3126,10 @@
         <v>0.02552106059786067</v>
       </c>
       <c r="H54">
-        <v>0.0646436933857772</v>
+        <v>0.01868847809710864</v>
       </c>
       <c r="I54">
-        <v>0.4513547050110129</v>
+        <v>0.4689854913270295</v>
       </c>
     </row>
     <row r="55">
@@ -2180,10 +3159,10 @@
         <v>0.7566432838732358</v>
       </c>
       <c r="H55">
-        <v>-0.179999481623082</v>
+        <v>-0.1473158358487471</v>
       </c>
       <c r="I55">
-        <v>0.2259427674730067</v>
+        <v>0.2490705241976982</v>
       </c>
     </row>
     <row r="56">
@@ -2213,10 +3192,10 @@
         <v>0.3049960550506722</v>
       </c>
       <c r="H56">
-        <v>-0.559860274345742</v>
+        <v>-0.5271390023140043</v>
       </c>
       <c r="I56">
-        <v>0.1911453236955528</v>
+        <v>0.1900741855111074</v>
       </c>
     </row>
     <row r="57">
@@ -2246,10 +3225,10 @@
         <v>0.09608970220299448</v>
       </c>
       <c r="H57">
-        <v>-0.5665630755051345</v>
+        <v>-0.6106246844115909</v>
       </c>
       <c r="I57">
-        <v>0.05936262993024379</v>
+        <v>0.1150691857279537</v>
       </c>
     </row>
     <row r="58">
@@ -2279,10 +3258,10 @@
         <v>0.842306744464044</v>
       </c>
       <c r="H58">
-        <v>-0.2457784186756974</v>
+        <v>-0.2179177176236429</v>
       </c>
       <c r="I58">
-        <v>0.2706523699594591</v>
+        <v>0.2577271737439232</v>
       </c>
     </row>
     <row r="59">
@@ -2312,10 +3291,10 @@
         <v>0.7441152366941269</v>
       </c>
       <c r="H59">
-        <v>-0.2747501239923872</v>
+        <v>-0.273389972613713</v>
       </c>
       <c r="I59">
-        <v>0.2205014879290451</v>
+        <v>0.2038469268489081</v>
       </c>
     </row>
     <row r="60">
@@ -2345,10 +3324,10 @@
         <v>0.235145350722716</v>
       </c>
       <c r="H60">
-        <v>-0.1679464565952759</v>
+        <v>-0.1783973998305011</v>
       </c>
       <c r="I60">
-        <v>0.7806778125284742</v>
+        <v>0.7375508758310919</v>
       </c>
     </row>
     <row r="61">
@@ -2378,10 +3357,10 @@
         <v>0.2951611497403613</v>
       </c>
       <c r="H61">
-        <v>-0.2162398675865032</v>
+        <v>-0.2450139390462626</v>
       </c>
       <c r="I61">
-        <v>0.707506653980175</v>
+        <v>0.7419979674033709</v>
       </c>
     </row>
     <row r="62">
@@ -2411,10 +3390,10 @@
         <v>0.6272295597475857</v>
       </c>
       <c r="H62">
-        <v>-0.4081007376825947</v>
+        <v>-0.391308173998236</v>
       </c>
       <c r="I62">
-        <v>0.2342909159300173</v>
+        <v>0.2162879109923399</v>
       </c>
     </row>
     <row r="63">
@@ -2444,10 +3423,10 @@
         <v>0.06795618094415351</v>
       </c>
       <c r="H63">
-        <v>0.2074747854129992</v>
+        <v>0.2670468805464514</v>
       </c>
       <c r="I63">
-        <v>1.664608077268614</v>
+        <v>1.648658946821268</v>
       </c>
     </row>
     <row r="64">
@@ -2477,10 +3456,10 @@
         <v>0.009074639437384492</v>
       </c>
       <c r="H64">
-        <v>0.3701678291626072</v>
+        <v>0.4156365575662241</v>
       </c>
       <c r="I64">
-        <v>2.218762328205875</v>
+        <v>2.213695008096214</v>
       </c>
     </row>
     <row r="65">
@@ -2510,10 +3489,10 @@
         <v>0.5346110040162471</v>
       </c>
       <c r="H65">
-        <v>-1.116997475197174</v>
+        <v>-1.018417461276735</v>
       </c>
       <c r="I65">
-        <v>0.573469732436428</v>
+        <v>0.5921911705357474</v>
       </c>
     </row>
     <row r="66">
@@ -2543,10 +3522,10 @@
         <v>0.9877876072461564</v>
       </c>
       <c r="H66">
-        <v>-0.7507702445197423</v>
+        <v>-0.7733914802293201</v>
       </c>
       <c r="I66">
-        <v>0.6822247161434973</v>
+        <v>0.7059403408282521</v>
       </c>
     </row>
     <row r="67">
@@ -2576,10 +3555,10 @@
         <v>0.7562129867133393</v>
       </c>
       <c r="H67">
-        <v>-0.5135042558740527</v>
+        <v>-0.5092390612477363</v>
       </c>
       <c r="I67">
-        <v>0.8065959384670668</v>
+        <v>0.7362541185173312</v>
       </c>
     </row>
     <row r="68">
@@ -2609,10 +3588,10 @@
         <v>0.4371199836563215</v>
       </c>
       <c r="H68">
-        <v>-0.9366237512805692</v>
+        <v>-0.954693347202311</v>
       </c>
       <c r="I68">
-        <v>0.4012326362462391</v>
+        <v>0.3965136817114013</v>
       </c>
     </row>
     <row r="69">
@@ -2642,10 +3621,10 @@
         <v>0.265975840793027</v>
       </c>
       <c r="H69">
-        <v>-1.080947469156825</v>
+        <v>-1.059301475802795</v>
       </c>
       <c r="I69">
-        <v>0.2687593865414813</v>
+        <v>0.2695508167836265</v>
       </c>
     </row>
     <row r="70">
@@ -2675,10 +3654,10 @@
         <v>0.6398161157351145</v>
       </c>
       <c r="H70">
-        <v>-1.202592891669766</v>
+        <v>-1.109858240496404</v>
       </c>
       <c r="I70">
-        <v>0.6895757891360447</v>
+        <v>0.6625868018510094</v>
       </c>
     </row>
     <row r="71">
@@ -2708,10 +3687,10 @@
         <v>0.1388774323826338</v>
       </c>
       <c r="H71">
-        <v>-1.730503086812985</v>
+        <v>-1.839443780815663</v>
       </c>
       <c r="I71">
-        <v>0.2112342808621257</v>
+        <v>0.1600168304493866</v>
       </c>
     </row>
     <row r="72">
@@ -2741,10 +3720,10 @@
         <v>0.02634303725309236</v>
       </c>
       <c r="H72">
-        <v>0.05676096173683864</v>
+        <v>0.04228531468250928</v>
       </c>
       <c r="I72">
-        <v>0.4602785956309432</v>
+        <v>0.4777474124495106</v>
       </c>
     </row>
     <row r="73">
@@ -2774,10 +3753,10 @@
         <v>0.6528467733077792</v>
       </c>
       <c r="H73">
-        <v>-0.1688743170352346</v>
+        <v>-0.1528559584179251</v>
       </c>
       <c r="I73">
-        <v>0.2504799782908996</v>
+        <v>0.2520196990402656</v>
       </c>
     </row>
     <row r="74">
@@ -2807,10 +3786,10 @@
         <v>0.4309713622733931</v>
       </c>
       <c r="H74">
-        <v>-0.4895630568629628</v>
+        <v>-0.498016461233066</v>
       </c>
       <c r="I74">
-        <v>0.2150613868029253</v>
+        <v>0.2349578631451038</v>
       </c>
     </row>
     <row r="75">
@@ -2840,10 +3819,10 @@
         <v>0.1437130633060289</v>
       </c>
       <c r="H75">
-        <v>-0.5152706059455788</v>
+        <v>-0.5570215821223329</v>
       </c>
       <c r="I75">
-        <v>0.1027810024559568</v>
+        <v>0.08069249897980944</v>
       </c>
     </row>
     <row r="76">
@@ -2873,10 +3852,10 @@
         <v>0.7620249842309224</v>
       </c>
       <c r="H76">
-        <v>-0.2120439254651824</v>
+        <v>-0.2131875601963859</v>
       </c>
       <c r="I76">
-        <v>0.3009884948355417</v>
+        <v>0.2929422996964876</v>
       </c>
     </row>
     <row r="77">
@@ -2906,10 +3885,10 @@
         <v>0.8451542964897799</v>
       </c>
       <c r="H77">
-        <v>-0.2827124850534812</v>
+        <v>-0.294924092274174</v>
       </c>
       <c r="I77">
-        <v>0.2394545207089611</v>
+        <v>0.2706789530235086</v>
       </c>
     </row>
     <row r="78">
@@ -2939,10 +3918,10 @@
         <v>0.1523339419669436</v>
       </c>
       <c r="H78">
-        <v>-0.1295215287120853</v>
+        <v>-0.1097243358231692</v>
       </c>
       <c r="I78">
-        <v>0.7898877024529614</v>
+        <v>0.8663762112352434</v>
       </c>
     </row>
     <row r="79">
@@ -2972,10 +3951,10 @@
         <v>0.1937140941682198</v>
       </c>
       <c r="H79">
-        <v>-0.1240891213302673</v>
+        <v>-0.1773560147948503</v>
       </c>
       <c r="I79">
-        <v>0.7879384475793324</v>
+        <v>0.8177453684261563</v>
       </c>
     </row>
     <row r="80">
@@ -3005,10 +3984,10 @@
         <v>0.6228892726074567</v>
       </c>
       <c r="H80">
-        <v>-0.4205095940553708</v>
+        <v>-0.4296229306767893</v>
       </c>
       <c r="I80">
-        <v>0.2515074393167959</v>
+        <v>0.2379964344476136</v>
       </c>
     </row>
     <row r="81">
@@ -3038,10 +4017,10 @@
         <v>0.07118266288120408</v>
       </c>
       <c r="H81">
-        <v>0.1382453218045925</v>
+        <v>0.126193033927761</v>
       </c>
       <c r="I81">
-        <v>1.759006487044377</v>
+        <v>1.613611012732815</v>
       </c>
     </row>
     <row r="82">
@@ -3071,10 +4050,10 @@
         <v>0.01388748569888324</v>
       </c>
       <c r="H82">
-        <v>0.3756222572866085</v>
+        <v>0.3859126340195999</v>
       </c>
       <c r="I82">
-        <v>2.209887932876863</v>
+        <v>2.225621703435895</v>
       </c>
     </row>
     <row r="83">
@@ -3104,10 +4083,10 @@
         <v>0.9818493285972396</v>
       </c>
       <c r="H83">
-        <v>-0.8034985602774655</v>
+        <v>-0.8468966571305967</v>
       </c>
       <c r="I83">
-        <v>0.8071375161446924</v>
+        <v>0.7955763038991264</v>
       </c>
     </row>
     <row r="84">
@@ -3137,10 +4116,10 @@
         <v>0.4921161866203829</v>
       </c>
       <c r="H84">
-        <v>-1.022838102785377</v>
+        <v>-1.038559087321565</v>
       </c>
       <c r="I84">
-        <v>0.4968156129822929</v>
+        <v>0.5274182481282809</v>
       </c>
     </row>
     <row r="85">
@@ -3170,10 +4149,10 @@
         <v>0.2428635814603371</v>
       </c>
       <c r="H85">
-        <v>-0.3845054548561551</v>
+        <v>-0.2638266670763103</v>
       </c>
       <c r="I85">
-        <v>1.170929174702328</v>
+        <v>1.254368967721135</v>
       </c>
     </row>
     <row r="86">
@@ -3203,10 +4182,10 @@
         <v>0.3836512004677323</v>
       </c>
       <c r="H86">
-        <v>-0.8946333851116295</v>
+        <v>-0.8897996273749877</v>
       </c>
       <c r="I86">
-        <v>0.3580436058466405</v>
+        <v>0.3673949261985546</v>
       </c>
     </row>
     <row r="87">
@@ -3236,10 +4215,10 @@
         <v>0.0622052216519151</v>
       </c>
       <c r="H87">
-        <v>-1.401655587490678</v>
+        <v>-1.351334649167237</v>
       </c>
       <c r="I87">
-        <v>0.01514190748543263</v>
+        <v>0.01353991027879861</v>
       </c>
     </row>
     <row r="88">
@@ -3269,10 +4248,10 @@
         <v>0.5665181571250247</v>
       </c>
       <c r="H88">
-        <v>-0.5033143858273386</v>
+        <v>-0.6459190534240458</v>
       </c>
       <c r="I88">
-        <v>0.9283960365373308</v>
+        <v>0.9950262694502696</v>
       </c>
     </row>
     <row r="89">
@@ -3302,10 +4281,10 @@
         <v>0.08874797797433839</v>
       </c>
       <c r="H89">
-        <v>-1.77650313269583</v>
+        <v>-1.784380427069038</v>
       </c>
       <c r="I89">
-        <v>0.1099384844683234</v>
+        <v>0.1368682417177456</v>
       </c>
     </row>
     <row r="90">
@@ -3335,10 +4314,10 @@
         <v>0.6805762752103817</v>
       </c>
       <c r="H90">
-        <v>-2.337708385121676</v>
+        <v>-2.32992515797036</v>
       </c>
       <c r="I90">
-        <v>1.494327743510744</v>
+        <v>1.595742731937204</v>
       </c>
     </row>
     <row r="91">
@@ -3368,10 +4347,10 @@
         <v>0.0171047475372586</v>
       </c>
       <c r="H91">
-        <v>0.03452454519930332</v>
+        <v>0.02944091275184552</v>
       </c>
       <c r="I91">
-        <v>0.4853486679163333</v>
+        <v>0.4880643081153995</v>
       </c>
     </row>
     <row r="92">
@@ -3401,10 +4380,10 @@
         <v>0.6294282350164404</v>
       </c>
       <c r="H92">
-        <v>-0.1394447162848179</v>
+        <v>-0.1233752667412616</v>
       </c>
       <c r="I92">
-        <v>0.2565184000887056</v>
+        <v>0.2512473549094</v>
       </c>
     </row>
     <row r="93">
@@ -3434,10 +4413,10 @@
         <v>0.3701775981872214</v>
       </c>
       <c r="H93">
-        <v>-0.5526898196041307</v>
+        <v>-0.530613310006274</v>
       </c>
       <c r="I93">
-        <v>0.1855472989589905</v>
+        <v>0.2158855366141342</v>
       </c>
     </row>
     <row r="94">
@@ -3467,10 +4446,10 @@
         <v>0.139803381922805</v>
       </c>
       <c r="H94">
-        <v>-0.5472319772728955</v>
+        <v>-0.5298817305154071</v>
       </c>
       <c r="I94">
-        <v>0.0552227649414335</v>
+        <v>0.08992892225687792</v>
       </c>
     </row>
     <row r="95">
@@ -3500,10 +4479,10 @@
         <v>0.6624447581429929</v>
       </c>
       <c r="H95">
-        <v>-0.1805359711526181</v>
+        <v>-0.1883575395310181</v>
       </c>
       <c r="I95">
-        <v>0.2750952613552468</v>
+        <v>0.3103465862379789</v>
       </c>
     </row>
     <row r="96">
@@ -3533,10 +4512,10 @@
         <v>0.5786196890687467</v>
       </c>
       <c r="H96">
-        <v>-0.3149813788461248</v>
+        <v>-0.3265829290471354</v>
       </c>
       <c r="I96">
-        <v>0.1621926726996425</v>
+        <v>0.189440859910058</v>
       </c>
     </row>
     <row r="97">
@@ -3566,10 +4545,10 @@
         <v>0.1127892657152508</v>
       </c>
       <c r="H97">
-        <v>-0.1437654873348643</v>
+        <v>-0.05384290292028718</v>
       </c>
       <c r="I97">
-        <v>0.8791652138308792</v>
+        <v>0.8940215039620572</v>
       </c>
     </row>
     <row r="98">
@@ -3599,10 +4578,10 @@
         <v>0.2308651827991921</v>
       </c>
       <c r="H98">
-        <v>-0.1817514105377187</v>
+        <v>-0.1435477302144261</v>
       </c>
       <c r="I98">
-        <v>0.7338935942432976</v>
+        <v>0.742717485758139</v>
       </c>
     </row>
     <row r="99">
@@ -3632,10 +4611,10 @@
         <v>0.6981069150025276</v>
       </c>
       <c r="H99">
-        <v>-0.3719236324210879</v>
+        <v>-0.367045117499148</v>
       </c>
       <c r="I99">
-        <v>0.2470788544926675</v>
+        <v>0.2831941820965727</v>
       </c>
     </row>
     <row r="100">
@@ -3665,10 +4644,10 @@
         <v>0.07211603824108859</v>
       </c>
       <c r="H100">
-        <v>0.1326708745093426</v>
+        <v>0.1765639377626398</v>
       </c>
       <c r="I100">
-        <v>1.734103377981928</v>
+        <v>1.681912618007223</v>
       </c>
     </row>
     <row r="101">
@@ -3698,10 +4677,10 @@
         <v>0.02751146176058817</v>
       </c>
       <c r="H101">
-        <v>0.2006598797179951</v>
+        <v>0.2267108023023583</v>
       </c>
       <c r="I101">
-        <v>2.209674662506051</v>
+        <v>2.097315315184563</v>
       </c>
     </row>
     <row r="102">
@@ -3731,10 +4710,10 @@
         <v>0.7534917579778402</v>
       </c>
       <c r="H102">
-        <v>-0.6268925503358652</v>
+        <v>-0.7018766702102054</v>
       </c>
       <c r="I102">
-        <v>0.9765774990234576</v>
+        <v>0.9630794658530171</v>
       </c>
     </row>
     <row r="103">
@@ -3764,10 +4743,10 @@
         <v>0.5307703167747249</v>
       </c>
       <c r="H103">
-        <v>-1.108570073099137</v>
+        <v>-1.018466260982793</v>
       </c>
       <c r="I103">
-        <v>0.5199248109342673</v>
+        <v>0.5300470310307088</v>
       </c>
     </row>
     <row r="104">
@@ -3797,10 +4776,10 @@
         <v>0.242025881918261</v>
       </c>
       <c r="H104">
-        <v>-0.2885218081969568</v>
+        <v>-0.4019500625167826</v>
       </c>
       <c r="I104">
-        <v>1.205745716470553</v>
+        <v>1.297772707873737</v>
       </c>
     </row>
     <row r="105">
@@ -3830,10 +4809,10 @@
         <v>0.5492871213138103</v>
       </c>
       <c r="H105">
-        <v>-0.8276153374484838</v>
+        <v>-0.8478385752598845</v>
       </c>
       <c r="I105">
-        <v>0.4110555547650871</v>
+        <v>0.3616001262894699</v>
       </c>
     </row>
     <row r="106">
@@ -3863,10 +4842,10 @@
         <v>0.0473281590668292</v>
       </c>
       <c r="H106">
-        <v>-1.450199929989077</v>
+        <v>-1.418009751638822</v>
       </c>
       <c r="I106">
-        <v>0.04438631459464637</v>
+        <v>-0.03258513390303176</v>
       </c>
     </row>
     <row r="107">
@@ -3896,10 +4875,10 @@
         <v>0.7523725831091722</v>
       </c>
       <c r="H107">
-        <v>-0.8631170300908456</v>
+        <v>-0.9875966512742398</v>
       </c>
       <c r="I107">
-        <v>0.6920423953104837</v>
+        <v>0.6735680927635478</v>
       </c>
     </row>
     <row r="108">
@@ -3929,10 +4908,10 @@
         <v>0.3504003569843512</v>
       </c>
       <c r="H108">
-        <v>-1.248070648095067</v>
+        <v>-1.313315865863578</v>
       </c>
       <c r="I108">
-        <v>0.4948130190546234</v>
+        <v>0.4137953462140581</v>
       </c>
     </row>
     <row r="109">
@@ -3962,10 +4941,10 @@
         <v>0.6346988782055155</v>
       </c>
       <c r="H109">
-        <v>-2.439194963055713</v>
+        <v>-2.437460196629877</v>
       </c>
       <c r="I109">
-        <v>1.352623967556079</v>
+        <v>1.407165274905132</v>
       </c>
     </row>
     <row r="110">
@@ -3995,10 +4974,10 @@
         <v>0.01974869830851809</v>
       </c>
       <c r="H110">
-        <v>0.05358797731380294</v>
+        <v>0.02978969450725753</v>
       </c>
       <c r="I110">
-        <v>0.467126339333513</v>
+        <v>0.489124140443395</v>
       </c>
     </row>
     <row r="111">
@@ -4028,10 +5007,10 @@
         <v>0.6286705771373422</v>
       </c>
       <c r="H111">
-        <v>-0.1429771450232186</v>
+        <v>-0.1553128179048896</v>
       </c>
       <c r="I111">
-        <v>0.2442984484184534</v>
+        <v>0.2685148109302758</v>
       </c>
     </row>
     <row r="112">
@@ -4061,10 +5040,10 @@
         <v>0.3483975151156963</v>
       </c>
       <c r="H112">
-        <v>-0.5133644522027708</v>
+        <v>-0.52054561397513</v>
       </c>
       <c r="I112">
-        <v>0.1850851447463366</v>
+        <v>0.1721453550390795</v>
       </c>
     </row>
     <row r="113">
@@ -4094,10 +5073,10 @@
         <v>0.1370219668729625</v>
       </c>
       <c r="H113">
-        <v>-0.5390866180758546</v>
+        <v>-0.542665934574395</v>
       </c>
       <c r="I113">
-        <v>0.0743236297414465</v>
+        <v>0.04560264121557969</v>
       </c>
     </row>
     <row r="114">
@@ -4127,10 +5106,10 @@
         <v>0.8483975000063533</v>
       </c>
       <c r="H114">
-        <v>-0.1856301210960243</v>
+        <v>-0.2218630059654358</v>
       </c>
       <c r="I114">
-        <v>0.2510297212273121</v>
+        <v>0.2640175889126602</v>
       </c>
     </row>
     <row r="115">
@@ -4160,10 +5139,10 @@
         <v>0.6591620961543974</v>
       </c>
       <c r="H115">
-        <v>-0.3189093190922731</v>
+        <v>-0.3243995875618235</v>
       </c>
       <c r="I115">
-        <v>0.2212769027764263</v>
+        <v>0.1772254771819326</v>
       </c>
     </row>
     <row r="116">
@@ -4193,10 +5172,10 @@
         <v>0.1874080374019437</v>
       </c>
       <c r="H116">
-        <v>-0.1363431195688723</v>
+        <v>-0.1369490432228248</v>
       </c>
       <c r="I116">
-        <v>0.829137252619777</v>
+        <v>0.7751567897546661</v>
       </c>
     </row>
     <row r="117">
@@ -4226,10 +5205,10 @@
         <v>0.3007686223458441</v>
       </c>
       <c r="H117">
-        <v>-0.2294805567666325</v>
+        <v>-0.192365016174924</v>
       </c>
       <c r="I117">
-        <v>0.7443872444165893</v>
+        <v>0.7214176267529373</v>
       </c>
     </row>
     <row r="118">
@@ -4259,10 +5238,10 @@
         <v>0.6717673897353145</v>
       </c>
       <c r="H118">
-        <v>-0.4014850321883327</v>
+        <v>-0.4378338193059346</v>
       </c>
       <c r="I118">
-        <v>0.291101973978087</v>
+        <v>0.2515514714750376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add appendix, references, update tables and text with all comments.
</commit_message>
<xml_diff>
--- a/cumulative_results.xlsx
+++ b/cumulative_results.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q118"/>
+  <dimension ref="A1:Q130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -471,10 +471,10 @@
         <v>0.04964264048460895</v>
       </c>
       <c r="H2">
-        <v>0.2862340954906926</v>
+        <v>0.2834120504218763</v>
       </c>
       <c r="I2">
-        <v>1.648967338964327</v>
+        <v>1.710330982814986</v>
       </c>
       <c r="J2">
         <v>16</v>
@@ -519,10 +519,10 @@
         <v>0.6028693164558701</v>
       </c>
       <c r="H3">
-        <v>-0.3856633561857863</v>
+        <v>-0.3797637711929017</v>
       </c>
       <c r="I3">
-        <v>0.7109394422838996</v>
+        <v>0.6949390264494599</v>
       </c>
       <c r="J3">
         <v>16</v>
@@ -567,10 +567,10 @@
         <v>0.386240323001902</v>
       </c>
       <c r="H4">
-        <v>-0.75872991513925</v>
+        <v>-0.7918839605521191</v>
       </c>
       <c r="I4">
-        <v>0.2683497172284998</v>
+        <v>0.3300495205443998</v>
       </c>
       <c r="J4">
         <v>16</v>
@@ -615,10 +615,10 @@
         <v>0.03659352146781997</v>
       </c>
       <c r="H5">
-        <v>-1.01890985232992</v>
+        <v>-1.059810369144379</v>
       </c>
       <c r="I5">
-        <v>0.04640187659852996</v>
+        <v>0.004334489455683389</v>
       </c>
       <c r="J5">
         <v>16</v>
@@ -663,10 +663,10 @@
         <v>0.02865195558438659</v>
       </c>
       <c r="H6">
-        <v>0.006562047272790326</v>
+        <v>0.01185891213076445</v>
       </c>
       <c r="I6">
-        <v>0.4529963286423255</v>
+        <v>0.4510146604231831</v>
       </c>
       <c r="J6">
         <v>16</v>
@@ -711,10 +711,10 @@
         <v>0.9448898796854626</v>
       </c>
       <c r="H7">
-        <v>-0.209186906951652</v>
+        <v>-0.1881801200518049</v>
       </c>
       <c r="I7">
-        <v>0.216223496922463</v>
+        <v>0.2278871344841083</v>
       </c>
       <c r="J7">
         <v>16</v>
@@ -759,10 +759,10 @@
         <v>0.2932670504991191</v>
       </c>
       <c r="H8">
-        <v>-0.5420026229208045</v>
+        <v>-0.5774358585009145</v>
       </c>
       <c r="I8">
-        <v>0.2049381797783333</v>
+        <v>0.1909169310499046</v>
       </c>
       <c r="J8">
         <v>16</v>
@@ -807,10 +807,10 @@
         <v>0.07750829082893188</v>
       </c>
       <c r="H9">
-        <v>-0.594090219936199</v>
+        <v>-0.6008543696275791</v>
       </c>
       <c r="I9">
-        <v>0.06775443910799996</v>
+        <v>0.02102239884936347</v>
       </c>
       <c r="J9">
         <v>16</v>
@@ -855,10 +855,10 @@
         <v>0.817717335487248</v>
       </c>
       <c r="H10">
-        <v>-0.2078895971868763</v>
+        <v>-0.1987530278136226</v>
       </c>
       <c r="I10">
-        <v>0.2758790143920343</v>
+        <v>0.2402125283496313</v>
       </c>
       <c r="J10">
         <v>16</v>
@@ -903,10 +903,10 @@
         <v>0.5634618251164623</v>
       </c>
       <c r="H11">
-        <v>-0.3303061346749652</v>
+        <v>-0.3441025997747367</v>
       </c>
       <c r="I11">
-        <v>0.1685190126524619</v>
+        <v>0.212602855966769</v>
       </c>
       <c r="J11">
         <v>16</v>
@@ -951,10 +951,10 @@
         <v>0.2400809627951311</v>
       </c>
       <c r="H12">
-        <v>-0.185218066585658</v>
+        <v>-0.2094689139795239</v>
       </c>
       <c r="I12">
-        <v>0.7447657300540489</v>
+        <v>0.7080914543682141</v>
       </c>
       <c r="J12">
         <v>16</v>
@@ -999,10 +999,10 @@
         <v>0.3064575649738183</v>
       </c>
       <c r="H13">
-        <v>-0.2038332389873086</v>
+        <v>-0.2118972728836294</v>
       </c>
       <c r="I13">
-        <v>0.7191129042648454</v>
+        <v>0.6859994500633758</v>
       </c>
       <c r="J13">
         <v>16</v>
@@ -1047,10 +1047,10 @@
         <v>0.6054857849294826</v>
       </c>
       <c r="H14">
-        <v>-0.4549225709284624</v>
+        <v>-0.4219594073253026</v>
       </c>
       <c r="I14">
-        <v>0.2208791779373557</v>
+        <v>0.3043565858790745</v>
       </c>
       <c r="J14">
         <v>16</v>
@@ -1095,10 +1095,10 @@
         <v>0.05812185553694306</v>
       </c>
       <c r="H15">
-        <v>0.3503323524768479</v>
+        <v>0.2845412020792215</v>
       </c>
       <c r="I15">
-        <v>1.678295774196313</v>
+        <v>1.688628675083661</v>
       </c>
       <c r="J15">
         <v>18</v>
@@ -1152,10 +1152,10 @@
         <v>0.004307415602908025</v>
       </c>
       <c r="H16">
-        <v>0.2954894333941566</v>
+        <v>0.3423474667853794</v>
       </c>
       <c r="I16">
-        <v>1.85059744763241</v>
+        <v>1.836228693313179</v>
       </c>
       <c r="J16">
         <v>18</v>
@@ -1209,10 +1209,10 @@
         <v>0.5155238728790634</v>
       </c>
       <c r="H17">
-        <v>-0.7993290502379676</v>
+        <v>-0.8217424239781287</v>
       </c>
       <c r="I17">
-        <v>0.3574556335416999</v>
+        <v>0.373917330041954</v>
       </c>
       <c r="J17">
         <v>18</v>
@@ -1266,10 +1266,10 @@
         <v>0.678039927149849</v>
       </c>
       <c r="H18">
-        <v>-0.65716948170628</v>
+        <v>-0.6460974383511378</v>
       </c>
       <c r="I18">
-        <v>0.4342156524684461</v>
+        <v>0.4299232990056411</v>
       </c>
       <c r="J18">
         <v>18</v>
@@ -1323,10 +1323,10 @@
         <v>0.4090643909381595</v>
       </c>
       <c r="H19">
-        <v>-0.8610621813422327</v>
+        <v>-0.7894788144458892</v>
       </c>
       <c r="I19">
-        <v>0.3128270876381522</v>
+        <v>0.3158699429736271</v>
       </c>
       <c r="J19">
         <v>18</v>
@@ -1380,10 +1380,10 @@
         <v>0.03279137701991269</v>
       </c>
       <c r="H20">
-        <v>-1.584011153275394</v>
+        <v>-1.566691695612505</v>
       </c>
       <c r="I20">
-        <v>-0.03264317216036437</v>
+        <v>-0.08708095587187574</v>
       </c>
       <c r="J20">
         <v>18</v>
@@ -1437,10 +1437,10 @@
         <v>0.02760057400643724</v>
       </c>
       <c r="H21">
-        <v>0.02458238190772083</v>
+        <v>0.03022460932315688</v>
       </c>
       <c r="I21">
-        <v>0.4529090083278975</v>
+        <v>0.4732341249810488</v>
       </c>
       <c r="J21">
         <v>18</v>
@@ -1494,10 +1494,10 @@
         <v>0.6799018601661131</v>
       </c>
       <c r="H22">
-        <v>-0.1604459511345854</v>
+        <v>-0.1363081466817822</v>
       </c>
       <c r="I22">
-        <v>0.2454738191131656</v>
+        <v>0.2407241054335687</v>
       </c>
       <c r="J22">
         <v>18</v>
@@ -1551,10 +1551,10 @@
         <v>0.3882036853072163</v>
       </c>
       <c r="H23">
-        <v>-0.4762321292867966</v>
+        <v>-0.5220301717860029</v>
       </c>
       <c r="I23">
-        <v>0.2121530345600002</v>
+        <v>0.2266035074830791</v>
       </c>
       <c r="J23">
         <v>18</v>
@@ -1608,10 +1608,10 @@
         <v>0.1670040167557344</v>
       </c>
       <c r="H24">
-        <v>-0.5390743257483683</v>
+        <v>-0.5366131893577966</v>
       </c>
       <c r="I24">
-        <v>0.08497938811892621</v>
+        <v>0.1201307121267209</v>
       </c>
       <c r="J24">
         <v>18</v>
@@ -1665,10 +1665,10 @@
         <v>0.9928509467147366</v>
       </c>
       <c r="H25">
-        <v>-0.2215532296616132</v>
+        <v>-0.2524642001192443</v>
       </c>
       <c r="I25">
-        <v>0.2444659215465013</v>
+        <v>0.230783945469051</v>
       </c>
       <c r="J25">
         <v>18</v>
@@ -1722,10 +1722,10 @@
         <v>0.789229887055815</v>
       </c>
       <c r="H26">
-        <v>-0.2844730655598888</v>
+        <v>-0.2919725654247182</v>
       </c>
       <c r="I26">
-        <v>0.198991600251633</v>
+        <v>0.223047941305191</v>
       </c>
       <c r="J26">
         <v>18</v>
@@ -1779,10 +1779,10 @@
         <v>0.325594064051256</v>
       </c>
       <c r="H27">
-        <v>-0.2821687751094802</v>
+        <v>-0.2615766894516497</v>
       </c>
       <c r="I27">
-        <v>0.688194791328801</v>
+        <v>0.7343499209923907</v>
       </c>
       <c r="J27">
         <v>18</v>
@@ -1836,10 +1836,10 @@
         <v>0.4106991278636435</v>
       </c>
       <c r="H28">
-        <v>-0.2407674385682356</v>
+        <v>-0.2948680693498724</v>
       </c>
       <c r="I28">
-        <v>0.6128732183646094</v>
+        <v>0.7000886864759898</v>
       </c>
       <c r="J28">
         <v>18</v>
@@ -1893,10 +1893,10 @@
         <v>0.4271125636813243</v>
       </c>
       <c r="H29">
-        <v>-0.4625301030330881</v>
+        <v>-0.4840510266555417</v>
       </c>
       <c r="I29">
-        <v>0.1911731166775313</v>
+        <v>0.198574693034343</v>
       </c>
       <c r="J29">
         <v>18</v>
@@ -1950,10 +1950,10 @@
         <v>0.06252292722425552</v>
       </c>
       <c r="H30">
-        <v>0.3125829819526447</v>
+        <v>0.2137330607612459</v>
       </c>
       <c r="I30">
-        <v>1.609924375241359</v>
+        <v>1.658602429560259</v>
       </c>
       <c r="J30">
         <v>19</v>
@@ -2007,10 +2007,10 @@
         <v>0.004849334745694508</v>
       </c>
       <c r="H31">
-        <v>0.33032748846421</v>
+        <v>0.3680090565890101</v>
       </c>
       <c r="I31">
-        <v>2.190418517249494</v>
+        <v>2.044476804175094</v>
       </c>
       <c r="J31">
         <v>19</v>
@@ -2064,10 +2064,10 @@
         <v>0.9186748126778145</v>
       </c>
       <c r="H32">
-        <v>-0.734644387179208</v>
+        <v>-0.693494691170524</v>
       </c>
       <c r="I32">
-        <v>0.6831429284207239</v>
+        <v>0.6586925022636354</v>
       </c>
       <c r="J32">
         <v>19</v>
@@ -2121,10 +2121,10 @@
         <v>0.4481234189980438</v>
       </c>
       <c r="H33">
-        <v>-0.7964892139021089</v>
+        <v>-0.7475689974832084</v>
       </c>
       <c r="I33">
-        <v>0.3066575248178697</v>
+        <v>0.3335766308591917</v>
       </c>
       <c r="J33">
         <v>19</v>
@@ -2178,10 +2178,10 @@
         <v>0.3671602410124577</v>
       </c>
       <c r="H34">
-        <v>-0.8396189919628324</v>
+        <v>-0.8877377064802509</v>
       </c>
       <c r="I34">
-        <v>0.2812554753050258</v>
+        <v>0.3115219482590851</v>
       </c>
       <c r="J34">
         <v>19</v>
@@ -2235,10 +2235,10 @@
         <v>0.7668946240781603</v>
       </c>
       <c r="H35">
-        <v>-0.7594545357787538</v>
+        <v>-0.744452479459231</v>
       </c>
       <c r="I35">
-        <v>0.5402843201127598</v>
+        <v>0.5511582570052165</v>
       </c>
       <c r="J35">
         <v>19</v>
@@ -2292,10 +2292,10 @@
         <v>0.03108283570422055</v>
       </c>
       <c r="H36">
-        <v>-1.738115458740259</v>
+        <v>-1.688749101184015</v>
       </c>
       <c r="I36">
-        <v>-0.04179908567843431</v>
+        <v>-0.09346320331169729</v>
       </c>
       <c r="J36">
         <v>19</v>
@@ -2349,10 +2349,10 @@
         <v>0.02175506015455142</v>
       </c>
       <c r="H37">
-        <v>0.01115372992588829</v>
+        <v>0.03604945668322138</v>
       </c>
       <c r="I37">
-        <v>0.4533302956142493</v>
+        <v>0.4662316548215919</v>
       </c>
       <c r="J37">
         <v>19</v>
@@ -2406,10 +2406,10 @@
         <v>0.6977696725009876</v>
       </c>
       <c r="H38">
-        <v>-0.1712367182825224</v>
+        <v>-0.1633368304452101</v>
       </c>
       <c r="I38">
-        <v>0.2455096365025987</v>
+        <v>0.230800896857949</v>
       </c>
       <c r="J38">
         <v>19</v>
@@ -2463,10 +2463,10 @@
         <v>0.3802621071032635</v>
       </c>
       <c r="H39">
-        <v>-0.5002049795210112</v>
+        <v>-0.5407540741261334</v>
       </c>
       <c r="I39">
-        <v>0.191529337971982</v>
+        <v>0.2049409166018693</v>
       </c>
       <c r="J39">
         <v>19</v>
@@ -2520,10 +2520,10 @@
         <v>0.1410514875989229</v>
       </c>
       <c r="H40">
-        <v>-0.5455031111243596</v>
+        <v>-0.5496273570798524</v>
       </c>
       <c r="I40">
-        <v>0.07736329385446518</v>
+        <v>0.06996570317065998</v>
       </c>
       <c r="J40">
         <v>19</v>
@@ -2577,10 +2577,10 @@
         <v>0.8959805637514762</v>
       </c>
       <c r="H41">
-        <v>-0.2028372948973302</v>
+        <v>-0.2242934259585204</v>
       </c>
       <c r="I41">
-        <v>0.2493083657628704</v>
+        <v>0.2682195949888659</v>
       </c>
       <c r="J41">
         <v>19</v>
@@ -2634,10 +2634,10 @@
         <v>0.68815076450387</v>
       </c>
       <c r="H42">
-        <v>-0.3218395372746429</v>
+        <v>-0.3293431498064522</v>
       </c>
       <c r="I42">
-        <v>0.2074403738074544</v>
+        <v>0.2180059070374321</v>
       </c>
       <c r="J42">
         <v>19</v>
@@ -2691,10 +2691,10 @@
         <v>0.2290822980262702</v>
       </c>
       <c r="H43">
-        <v>-0.1985776008259142</v>
+        <v>-0.1532693840751618</v>
       </c>
       <c r="I43">
-        <v>0.765280334170213</v>
+        <v>0.76705513253247</v>
       </c>
       <c r="J43">
         <v>19</v>
@@ -2748,10 +2748,10 @@
         <v>0.2501239398540214</v>
       </c>
       <c r="H44">
-        <v>-0.1785622044193332</v>
+        <v>-0.1700613969589585</v>
       </c>
       <c r="I44">
-        <v>0.7211604152695491</v>
+        <v>0.7246833565176921</v>
       </c>
       <c r="J44">
         <v>19</v>
@@ -2805,10 +2805,10 @@
         <v>0.4913382811027023</v>
       </c>
       <c r="H45">
-        <v>-0.4165754255433853</v>
+        <v>-0.412485709777026</v>
       </c>
       <c r="I45">
-        <v>0.2152630253709437</v>
+        <v>0.2035585290045968</v>
       </c>
       <c r="J45">
         <v>19</v>
@@ -2862,10 +2862,10 @@
         <v>0.06297009607337689</v>
       </c>
       <c r="H46">
-        <v>0.155808429375246</v>
+        <v>0.2986598028976839</v>
       </c>
       <c r="I46">
-        <v>1.622986304153297</v>
+        <v>1.629211434857524</v>
       </c>
     </row>
     <row r="47">
@@ -2895,10 +2895,10 @@
         <v>0.005049185733957656</v>
       </c>
       <c r="H47">
-        <v>0.4079785539316004</v>
+        <v>0.2653809009916422</v>
       </c>
       <c r="I47">
-        <v>2.027418079898665</v>
+        <v>1.984193583738628</v>
       </c>
     </row>
     <row r="48">
@@ -2928,10 +2928,10 @@
         <v>0.8637447796552011</v>
       </c>
       <c r="H48">
-        <v>-0.7665783931071387</v>
+        <v>-0.8982748920281581</v>
       </c>
       <c r="I48">
-        <v>0.6853448030848063</v>
+        <v>0.7412443534161096</v>
       </c>
     </row>
     <row r="49">
@@ -2961,10 +2961,10 @@
         <v>0.7142314729337769</v>
       </c>
       <c r="H49">
-        <v>-0.6142831104819919</v>
+        <v>-0.4954934610532872</v>
       </c>
       <c r="I49">
-        <v>0.7710330737280957</v>
+        <v>0.7356696601534916</v>
       </c>
     </row>
     <row r="50">
@@ -2994,10 +2994,10 @@
         <v>0.409779029170831</v>
       </c>
       <c r="H50">
-        <v>-0.7507291499353248</v>
+        <v>-0.792303563299306</v>
       </c>
       <c r="I50">
-        <v>0.3442006450209224</v>
+        <v>0.3651950463291019</v>
       </c>
     </row>
     <row r="51">
@@ -3027,10 +3027,10 @@
         <v>0.5970401227461903</v>
       </c>
       <c r="H51">
-        <v>-0.8687266060483141</v>
+        <v>-0.8841391112961295</v>
       </c>
       <c r="I51">
-        <v>0.5070316976568988</v>
+        <v>0.5331176113778089</v>
       </c>
     </row>
     <row r="52">
@@ -3060,10 +3060,10 @@
         <v>0.2563739878656627</v>
       </c>
       <c r="H52">
-        <v>-1.103917488190971</v>
+        <v>-1.11267580902433</v>
       </c>
       <c r="I52">
-        <v>0.3163342809448065</v>
+        <v>0.2868962243083319</v>
       </c>
     </row>
     <row r="53">
@@ -3093,10 +3093,10 @@
         <v>0.1452463571798465</v>
       </c>
       <c r="H53">
-        <v>-1.721754345843732</v>
+        <v>-1.870352304635462</v>
       </c>
       <c r="I53">
-        <v>0.264307641549676</v>
+        <v>0.33845646276466</v>
       </c>
     </row>
     <row r="54">
@@ -3126,10 +3126,10 @@
         <v>0.02552106059786067</v>
       </c>
       <c r="H54">
-        <v>0.01868847809710864</v>
+        <v>0.01683720703488287</v>
       </c>
       <c r="I54">
-        <v>0.4689854913270295</v>
+        <v>0.463454810334081</v>
       </c>
     </row>
     <row r="55">
@@ -3159,10 +3159,10 @@
         <v>0.7566432838732358</v>
       </c>
       <c r="H55">
-        <v>-0.1473158358487471</v>
+        <v>-0.1701932528374098</v>
       </c>
       <c r="I55">
-        <v>0.2490705241976982</v>
+        <v>0.2279255872861863</v>
       </c>
     </row>
     <row r="56">
@@ -3192,10 +3192,10 @@
         <v>0.3049960550506722</v>
       </c>
       <c r="H56">
-        <v>-0.5271390023140043</v>
+        <v>-0.5345250188439093</v>
       </c>
       <c r="I56">
-        <v>0.1900741855111074</v>
+        <v>0.1751483894405875</v>
       </c>
     </row>
     <row r="57">
@@ -3225,10 +3225,10 @@
         <v>0.09608970220299448</v>
       </c>
       <c r="H57">
-        <v>-0.6106246844115909</v>
+        <v>-0.5733178913008012</v>
       </c>
       <c r="I57">
-        <v>0.1150691857279537</v>
+        <v>0.05632603982299498</v>
       </c>
     </row>
     <row r="58">
@@ -3258,10 +3258,10 @@
         <v>0.842306744464044</v>
       </c>
       <c r="H58">
-        <v>-0.2179177176236429</v>
+        <v>-0.2423031895720431</v>
       </c>
       <c r="I58">
-        <v>0.2577271737439232</v>
+        <v>0.2648156129668164</v>
       </c>
     </row>
     <row r="59">
@@ -3291,10 +3291,10 @@
         <v>0.7441152366941269</v>
       </c>
       <c r="H59">
-        <v>-0.273389972613713</v>
+        <v>-0.2945602548646099</v>
       </c>
       <c r="I59">
-        <v>0.2038469268489081</v>
+        <v>0.2341668538710682</v>
       </c>
     </row>
     <row r="60">
@@ -3324,10 +3324,10 @@
         <v>0.235145350722716</v>
       </c>
       <c r="H60">
-        <v>-0.1783973998305011</v>
+        <v>-0.2129792590129806</v>
       </c>
       <c r="I60">
-        <v>0.7375508758310919</v>
+        <v>0.7971000428529461</v>
       </c>
     </row>
     <row r="61">
@@ -3357,10 +3357,10 @@
         <v>0.2951611497403613</v>
       </c>
       <c r="H61">
-        <v>-0.2450139390462626</v>
+        <v>-0.2227848257188881</v>
       </c>
       <c r="I61">
-        <v>0.7419979674033709</v>
+        <v>0.6232356320231051</v>
       </c>
     </row>
     <row r="62">
@@ -3390,10 +3390,10 @@
         <v>0.6272295597475857</v>
       </c>
       <c r="H62">
-        <v>-0.391308173998236</v>
+        <v>-0.3990319561571715</v>
       </c>
       <c r="I62">
-        <v>0.2162879109923399</v>
+        <v>0.2562634182084488</v>
       </c>
     </row>
     <row r="63">
@@ -3423,10 +3423,10 @@
         <v>0.06795618094415351</v>
       </c>
       <c r="H63">
-        <v>0.2670468805464514</v>
+        <v>0.2323931087977209</v>
       </c>
       <c r="I63">
-        <v>1.648658946821268</v>
+        <v>1.576632022519839</v>
       </c>
     </row>
     <row r="64">
@@ -3456,10 +3456,10 @@
         <v>0.009074639437384492</v>
       </c>
       <c r="H64">
-        <v>0.4156365575662241</v>
+        <v>0.3128768293263516</v>
       </c>
       <c r="I64">
-        <v>2.213695008096214</v>
+        <v>2.138696556873741</v>
       </c>
     </row>
     <row r="65">
@@ -3489,10 +3489,10 @@
         <v>0.5346110040162471</v>
       </c>
       <c r="H65">
-        <v>-1.018417461276735</v>
+        <v>-1.078233440312897</v>
       </c>
       <c r="I65">
-        <v>0.5921911705357474</v>
+        <v>0.619058509602279</v>
       </c>
     </row>
     <row r="66">
@@ -3522,10 +3522,10 @@
         <v>0.9877876072461564</v>
       </c>
       <c r="H66">
-        <v>-0.7733914802293201</v>
+        <v>-0.7695640373869607</v>
       </c>
       <c r="I66">
-        <v>0.7059403408282521</v>
+        <v>0.6675427985893866</v>
       </c>
     </row>
     <row r="67">
@@ -3555,10 +3555,10 @@
         <v>0.7562129867133393</v>
       </c>
       <c r="H67">
-        <v>-0.5092390612477363</v>
+        <v>-0.5166593623343072</v>
       </c>
       <c r="I67">
-        <v>0.7362541185173312</v>
+        <v>0.7407831192271974</v>
       </c>
     </row>
     <row r="68">
@@ -3588,10 +3588,10 @@
         <v>0.4371199836563215</v>
       </c>
       <c r="H68">
-        <v>-0.954693347202311</v>
+        <v>-0.8950902909756037</v>
       </c>
       <c r="I68">
-        <v>0.3965136817114013</v>
+        <v>0.3932120204458459</v>
       </c>
     </row>
     <row r="69">
@@ -3621,10 +3621,10 @@
         <v>0.265975840793027</v>
       </c>
       <c r="H69">
-        <v>-1.059301475802795</v>
+        <v>-1.079929917376834</v>
       </c>
       <c r="I69">
-        <v>0.2695508167836265</v>
+        <v>0.2910029782468126</v>
       </c>
     </row>
     <row r="70">
@@ -3654,10 +3654,10 @@
         <v>0.6398161157351145</v>
       </c>
       <c r="H70">
-        <v>-1.109858240496404</v>
+        <v>-1.07898417987663</v>
       </c>
       <c r="I70">
-        <v>0.6625868018510094</v>
+        <v>0.7463088327471763</v>
       </c>
     </row>
     <row r="71">
@@ -3687,10 +3687,10 @@
         <v>0.1388774323826338</v>
       </c>
       <c r="H71">
-        <v>-1.839443780815663</v>
+        <v>-1.828140024691209</v>
       </c>
       <c r="I71">
-        <v>0.1600168304493866</v>
+        <v>0.3069567228086447</v>
       </c>
     </row>
     <row r="72">
@@ -3720,10 +3720,10 @@
         <v>0.02634303725309236</v>
       </c>
       <c r="H72">
-        <v>0.04228531468250928</v>
+        <v>0.03596144205160846</v>
       </c>
       <c r="I72">
-        <v>0.4777474124495106</v>
+        <v>0.4639996784794094</v>
       </c>
     </row>
     <row r="73">
@@ -3753,10 +3753,10 @@
         <v>0.6528467733077792</v>
       </c>
       <c r="H73">
-        <v>-0.1528559584179251</v>
+        <v>-0.1743682744101016</v>
       </c>
       <c r="I73">
-        <v>0.2520196990402656</v>
+        <v>0.274024154047829</v>
       </c>
     </row>
     <row r="74">
@@ -3786,10 +3786,10 @@
         <v>0.4309713622733931</v>
       </c>
       <c r="H74">
-        <v>-0.498016461233066</v>
+        <v>-0.5227924949496681</v>
       </c>
       <c r="I74">
-        <v>0.2349578631451038</v>
+        <v>0.2049527346144591</v>
       </c>
     </row>
     <row r="75">
@@ -3819,10 +3819,10 @@
         <v>0.1437130633060289</v>
       </c>
       <c r="H75">
-        <v>-0.5570215821223329</v>
+        <v>-0.5533981237727951</v>
       </c>
       <c r="I75">
-        <v>0.08069249897980944</v>
+        <v>0.075477905957581</v>
       </c>
     </row>
     <row r="76">
@@ -3852,10 +3852,10 @@
         <v>0.7620249842309224</v>
       </c>
       <c r="H76">
-        <v>-0.2131875601963859</v>
+        <v>-0.188688170967089</v>
       </c>
       <c r="I76">
-        <v>0.2929422996964876</v>
+        <v>0.269750450751371</v>
       </c>
     </row>
     <row r="77">
@@ -3885,10 +3885,10 @@
         <v>0.8451542964897799</v>
       </c>
       <c r="H77">
-        <v>-0.294924092274174</v>
+        <v>-0.2991940213788358</v>
       </c>
       <c r="I77">
-        <v>0.2706789530235086</v>
+        <v>0.234207343157654</v>
       </c>
     </row>
     <row r="78">
@@ -3918,10 +3918,10 @@
         <v>0.1523339419669436</v>
       </c>
       <c r="H78">
-        <v>-0.1097243358231692</v>
+        <v>-0.1065578596107732</v>
       </c>
       <c r="I78">
-        <v>0.8663762112352434</v>
+        <v>0.7964343676736534</v>
       </c>
     </row>
     <row r="79">
@@ -3951,10 +3951,10 @@
         <v>0.1937140941682198</v>
       </c>
       <c r="H79">
-        <v>-0.1773560147948503</v>
+        <v>-0.1316507814749432</v>
       </c>
       <c r="I79">
-        <v>0.8177453684261563</v>
+        <v>0.7428793033540159</v>
       </c>
     </row>
     <row r="80">
@@ -3984,10 +3984,10 @@
         <v>0.6228892726074567</v>
       </c>
       <c r="H80">
-        <v>-0.4296229306767893</v>
+        <v>-0.4258892403898292</v>
       </c>
       <c r="I80">
-        <v>0.2379964344476136</v>
+        <v>0.2322929870432801</v>
       </c>
     </row>
     <row r="81">
@@ -4017,10 +4017,10 @@
         <v>0.07118266288120408</v>
       </c>
       <c r="H81">
-        <v>0.126193033927761</v>
+        <v>0.2673111094425235</v>
       </c>
       <c r="I81">
-        <v>1.613611012732815</v>
+        <v>1.719485347296794</v>
       </c>
     </row>
     <row r="82">
@@ -4050,10 +4050,10 @@
         <v>0.01388748569888324</v>
       </c>
       <c r="H82">
-        <v>0.3859126340195999</v>
+        <v>0.222364395750175</v>
       </c>
       <c r="I82">
-        <v>2.225621703435895</v>
+        <v>2.158108299591714</v>
       </c>
     </row>
     <row r="83">
@@ -4083,10 +4083,10 @@
         <v>0.9818493285972396</v>
       </c>
       <c r="H83">
-        <v>-0.8468966571305967</v>
+        <v>-0.8557526486193839</v>
       </c>
       <c r="I83">
-        <v>0.7955763038991264</v>
+        <v>0.8171297744621602</v>
       </c>
     </row>
     <row r="84">
@@ -4116,10 +4116,10 @@
         <v>0.4921161866203829</v>
       </c>
       <c r="H84">
-        <v>-1.038559087321565</v>
+        <v>-1.007918257285262</v>
       </c>
       <c r="I84">
-        <v>0.5274182481282809</v>
+        <v>0.3982341580861368</v>
       </c>
     </row>
     <row r="85">
@@ -4149,10 +4149,10 @@
         <v>0.2428635814603371</v>
       </c>
       <c r="H85">
-        <v>-0.2638266670763103</v>
+        <v>-0.394720525716212</v>
       </c>
       <c r="I85">
-        <v>1.254368967721135</v>
+        <v>1.137778952847658</v>
       </c>
     </row>
     <row r="86">
@@ -4182,10 +4182,10 @@
         <v>0.3836512004677323</v>
       </c>
       <c r="H86">
-        <v>-0.8897996273749877</v>
+        <v>-0.9247136587627589</v>
       </c>
       <c r="I86">
-        <v>0.3673949261985546</v>
+        <v>0.324190129806607</v>
       </c>
     </row>
     <row r="87">
@@ -4215,10 +4215,10 @@
         <v>0.0622052216519151</v>
       </c>
       <c r="H87">
-        <v>-1.351334649167237</v>
+        <v>-1.412294366105705</v>
       </c>
       <c r="I87">
-        <v>0.01353991027879861</v>
+        <v>0.01800030821982512</v>
       </c>
     </row>
     <row r="88">
@@ -4248,10 +4248,10 @@
         <v>0.5665181571250247</v>
       </c>
       <c r="H88">
-        <v>-0.6459190534240458</v>
+        <v>-0.561902816653414</v>
       </c>
       <c r="I88">
-        <v>0.9950262694502696</v>
+        <v>1.05319520517475</v>
       </c>
     </row>
     <row r="89">
@@ -4281,10 +4281,10 @@
         <v>0.08874797797433839</v>
       </c>
       <c r="H89">
-        <v>-1.784380427069038</v>
+        <v>-1.746891627418626</v>
       </c>
       <c r="I89">
-        <v>0.1368682417177456</v>
+        <v>0.1057977920009807</v>
       </c>
     </row>
     <row r="90">
@@ -4314,10 +4314,10 @@
         <v>0.6805762752103817</v>
       </c>
       <c r="H90">
-        <v>-2.32992515797036</v>
+        <v>-2.243477998319585</v>
       </c>
       <c r="I90">
-        <v>1.595742731937204</v>
+        <v>1.334353334209698</v>
       </c>
     </row>
     <row r="91">
@@ -4347,10 +4347,10 @@
         <v>0.0171047475372586</v>
       </c>
       <c r="H91">
-        <v>0.02944091275184552</v>
+        <v>0.03131807964961131</v>
       </c>
       <c r="I91">
-        <v>0.4880643081153995</v>
+        <v>0.4856834178222433</v>
       </c>
     </row>
     <row r="92">
@@ -4380,10 +4380,10 @@
         <v>0.6294282350164404</v>
       </c>
       <c r="H92">
-        <v>-0.1233752667412616</v>
+        <v>-0.1474607811314075</v>
       </c>
       <c r="I92">
-        <v>0.2512473549094</v>
+        <v>0.2749037543227097</v>
       </c>
     </row>
     <row r="93">
@@ -4413,10 +4413,10 @@
         <v>0.3701775981872214</v>
       </c>
       <c r="H93">
-        <v>-0.530613310006274</v>
+        <v>-0.4955892032030743</v>
       </c>
       <c r="I93">
-        <v>0.2158855366141342</v>
+        <v>0.1820975338784321</v>
       </c>
     </row>
     <row r="94">
@@ -4446,10 +4446,10 @@
         <v>0.139803381922805</v>
       </c>
       <c r="H94">
-        <v>-0.5298817305154071</v>
+        <v>-0.5134523786636653</v>
       </c>
       <c r="I94">
-        <v>0.08992892225687792</v>
+        <v>0.08377036447647154</v>
       </c>
     </row>
     <row r="95">
@@ -4479,10 +4479,10 @@
         <v>0.6624447581429929</v>
       </c>
       <c r="H95">
-        <v>-0.1883575395310181</v>
+        <v>-0.1780608891896219</v>
       </c>
       <c r="I95">
-        <v>0.3103465862379789</v>
+        <v>0.2926234428601105</v>
       </c>
     </row>
     <row r="96">
@@ -4512,10 +4512,10 @@
         <v>0.5786196890687467</v>
       </c>
       <c r="H96">
-        <v>-0.3265829290471354</v>
+        <v>-0.3342968566753575</v>
       </c>
       <c r="I96">
-        <v>0.189440859910058</v>
+        <v>0.2221274158816584</v>
       </c>
     </row>
     <row r="97">
@@ -4545,10 +4545,10 @@
         <v>0.1127892657152508</v>
       </c>
       <c r="H97">
-        <v>-0.05384290292028718</v>
+        <v>-0.0671744464590317</v>
       </c>
       <c r="I97">
-        <v>0.8940215039620572</v>
+        <v>0.9136146743299711</v>
       </c>
     </row>
     <row r="98">
@@ -4578,10 +4578,10 @@
         <v>0.2308651827991921</v>
       </c>
       <c r="H98">
-        <v>-0.1435477302144261</v>
+        <v>-0.1526611313382874</v>
       </c>
       <c r="I98">
-        <v>0.742717485758139</v>
+        <v>0.7246578534937453</v>
       </c>
     </row>
     <row r="99">
@@ -4611,10 +4611,10 @@
         <v>0.6981069150025276</v>
       </c>
       <c r="H99">
-        <v>-0.367045117499148</v>
+        <v>-0.4198854714730326</v>
       </c>
       <c r="I99">
-        <v>0.2831941820965727</v>
+        <v>0.2414114597236318</v>
       </c>
     </row>
     <row r="100">
@@ -4644,10 +4644,10 @@
         <v>0.07211603824108859</v>
       </c>
       <c r="H100">
-        <v>0.1765639377626398</v>
+        <v>0.2725837655375069</v>
       </c>
       <c r="I100">
-        <v>1.681912618007223</v>
+        <v>1.777996182182988</v>
       </c>
     </row>
     <row r="101">
@@ -4677,10 +4677,10 @@
         <v>0.02751146176058817</v>
       </c>
       <c r="H101">
-        <v>0.2267108023023583</v>
+        <v>0.1317889417820924</v>
       </c>
       <c r="I101">
-        <v>2.097315315184563</v>
+        <v>2.090994651440531</v>
       </c>
     </row>
     <row r="102">
@@ -4710,10 +4710,10 @@
         <v>0.7534917579778402</v>
       </c>
       <c r="H102">
-        <v>-0.7018766702102054</v>
+        <v>-0.624456053854468</v>
       </c>
       <c r="I102">
-        <v>0.9630794658530171</v>
+        <v>0.9422131521187354</v>
       </c>
     </row>
     <row r="103">
@@ -4743,10 +4743,10 @@
         <v>0.5307703167747249</v>
       </c>
       <c r="H103">
-        <v>-1.018466260982793</v>
+        <v>-1.022343971338151</v>
       </c>
       <c r="I103">
-        <v>0.5300470310307088</v>
+        <v>0.4638854161647995</v>
       </c>
     </row>
     <row r="104">
@@ -4776,10 +4776,10 @@
         <v>0.242025881918261</v>
       </c>
       <c r="H104">
-        <v>-0.4019500625167826</v>
+        <v>-0.3779898069407092</v>
       </c>
       <c r="I104">
-        <v>1.297772707873737</v>
+        <v>1.325995282193734</v>
       </c>
     </row>
     <row r="105">
@@ -4809,10 +4809,10 @@
         <v>0.5492871213138103</v>
       </c>
       <c r="H105">
-        <v>-0.8478385752598845</v>
+        <v>-0.8589683882192437</v>
       </c>
       <c r="I105">
-        <v>0.3616001262894699</v>
+        <v>0.3727335523255995</v>
       </c>
     </row>
     <row r="106">
@@ -4842,10 +4842,10 @@
         <v>0.0473281590668292</v>
       </c>
       <c r="H106">
-        <v>-1.418009751638822</v>
+        <v>-1.365660203976276</v>
       </c>
       <c r="I106">
-        <v>-0.03258513390303176</v>
+        <v>0.00253732698575367</v>
       </c>
     </row>
     <row r="107">
@@ -4875,10 +4875,10 @@
         <v>0.7523725831091722</v>
       </c>
       <c r="H107">
-        <v>-0.9875966512742398</v>
+        <v>-0.869175008089617</v>
       </c>
       <c r="I107">
-        <v>0.6735680927635478</v>
+        <v>0.6492382630557306</v>
       </c>
     </row>
     <row r="108">
@@ -4908,10 +4908,10 @@
         <v>0.3504003569843512</v>
       </c>
       <c r="H108">
-        <v>-1.313315865863578</v>
+        <v>-1.230602945337019</v>
       </c>
       <c r="I108">
-        <v>0.4137953462140581</v>
+        <v>0.53945142598191</v>
       </c>
     </row>
     <row r="109">
@@ -4941,10 +4941,10 @@
         <v>0.6346988782055155</v>
       </c>
       <c r="H109">
-        <v>-2.437460196629877</v>
+        <v>-2.429158278976642</v>
       </c>
       <c r="I109">
-        <v>1.407165274905132</v>
+        <v>1.478938348401716</v>
       </c>
     </row>
     <row r="110">
@@ -4974,10 +4974,10 @@
         <v>0.01974869830851809</v>
       </c>
       <c r="H110">
-        <v>0.02978969450725753</v>
+        <v>0.03935387375506106</v>
       </c>
       <c r="I110">
-        <v>0.489124140443395</v>
+        <v>0.4920917820816467</v>
       </c>
     </row>
     <row r="111">
@@ -5007,10 +5007,10 @@
         <v>0.6286705771373422</v>
       </c>
       <c r="H111">
-        <v>-0.1553128179048896</v>
+        <v>-0.1568214695319474</v>
       </c>
       <c r="I111">
-        <v>0.2685148109302758</v>
+        <v>0.2711518701597906</v>
       </c>
     </row>
     <row r="112">
@@ -5040,10 +5040,10 @@
         <v>0.3483975151156963</v>
       </c>
       <c r="H112">
-        <v>-0.52054561397513</v>
+        <v>-0.5272868128691247</v>
       </c>
       <c r="I112">
-        <v>0.1721453550390795</v>
+        <v>0.194056023203209</v>
       </c>
     </row>
     <row r="113">
@@ -5073,10 +5073,10 @@
         <v>0.1370219668729625</v>
       </c>
       <c r="H113">
-        <v>-0.542665934574395</v>
+        <v>-0.5395442905426656</v>
       </c>
       <c r="I113">
-        <v>0.04560264121557969</v>
+        <v>0.08028599407284376</v>
       </c>
     </row>
     <row r="114">
@@ -5106,10 +5106,10 @@
         <v>0.8483975000063533</v>
       </c>
       <c r="H114">
-        <v>-0.2218630059654358</v>
+        <v>-0.2489568335965543</v>
       </c>
       <c r="I114">
-        <v>0.2640175889126602</v>
+        <v>0.2545426214062962</v>
       </c>
     </row>
     <row r="115">
@@ -5139,10 +5139,10 @@
         <v>0.6591620961543974</v>
       </c>
       <c r="H115">
-        <v>-0.3243995875618235</v>
+        <v>-0.3162605634835158</v>
       </c>
       <c r="I115">
-        <v>0.1772254771819326</v>
+        <v>0.1888629570821694</v>
       </c>
     </row>
     <row r="116">
@@ -5172,10 +5172,10 @@
         <v>0.1874080374019437</v>
       </c>
       <c r="H116">
-        <v>-0.1369490432228248</v>
+        <v>-0.1616647097704486</v>
       </c>
       <c r="I116">
-        <v>0.7751567897546661</v>
+        <v>0.8008176094777707</v>
       </c>
     </row>
     <row r="117">
@@ -5205,10 +5205,10 @@
         <v>0.3007686223458441</v>
       </c>
       <c r="H117">
-        <v>-0.192365016174924</v>
+        <v>-0.223509098540499</v>
       </c>
       <c r="I117">
-        <v>0.7214176267529373</v>
+        <v>0.7052488566431703</v>
       </c>
     </row>
     <row r="118">
@@ -5238,10 +5238,406 @@
         <v>0.6717673897353145</v>
       </c>
       <c r="H118">
-        <v>-0.4378338193059346</v>
+        <v>-0.3462840722735976</v>
       </c>
       <c r="I118">
-        <v>0.2515514714750376</v>
+        <v>0.2618725088773809</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>final</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>(Intercept)</t>
+        </is>
+      </c>
+      <c r="C119">
+        <v>1.007273339280702</v>
+      </c>
+      <c r="D119">
+        <v>0.3501999357497746</v>
+      </c>
+      <c r="E119">
+        <v>3.172470899198462</v>
+      </c>
+      <c r="F119">
+        <v>2.876280765512248</v>
+      </c>
+      <c r="G119">
+        <v>0.05960262529393068</v>
+      </c>
+      <c r="H119">
+        <v>0.3344572786538703</v>
+      </c>
+      <c r="I119">
+        <v>1.670785315256443</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>final</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>ss3</t>
+        </is>
+      </c>
+      <c r="C120">
+        <v>-0.3189595705384181</v>
+      </c>
+      <c r="D120">
+        <v>0.2847241419242772</v>
+      </c>
+      <c r="E120">
+        <v>308.4388180221065</v>
+      </c>
+      <c r="F120">
+        <v>-1.12024069466946</v>
+      </c>
+      <c r="G120">
+        <v>0.2634827249448746</v>
+      </c>
+      <c r="H120">
+        <v>-0.8702382115366435</v>
+      </c>
+      <c r="I120">
+        <v>0.2592553230240116</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>final</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>ss5</t>
+        </is>
+      </c>
+      <c r="C121">
+        <v>-0.9330978595663808</v>
+      </c>
+      <c r="D121">
+        <v>0.3887967269619108</v>
+      </c>
+      <c r="E121">
+        <v>310.629643970146</v>
+      </c>
+      <c r="F121">
+        <v>-2.399963258069797</v>
+      </c>
+      <c r="G121">
+        <v>0.01698513286308198</v>
+      </c>
+      <c r="H121">
+        <v>-1.690428423429527</v>
+      </c>
+      <c r="I121">
+        <v>-0.1083078895178104</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>final</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>percenttwoormoreraces</t>
+        </is>
+      </c>
+      <c r="C122">
+        <v>0.2497937783222982</v>
+      </c>
+      <c r="D122">
+        <v>0.1096569986592566</v>
+      </c>
+      <c r="E122">
+        <v>314.8324654261288</v>
+      </c>
+      <c r="F122">
+        <v>2.277955637820223</v>
+      </c>
+      <c r="G122">
+        <v>0.02339915359643622</v>
+      </c>
+      <c r="H122">
+        <v>0.04079408245403552</v>
+      </c>
+      <c r="I122">
+        <v>0.4660123699072622</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>final</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>percentasian</t>
+        </is>
+      </c>
+      <c r="C123">
+        <v>0.002823085931828985</v>
+      </c>
+      <c r="D123">
+        <v>0.1053894874774536</v>
+      </c>
+      <c r="E123">
+        <v>308.8848183191699</v>
+      </c>
+      <c r="F123">
+        <v>0.0267871682404086</v>
+      </c>
+      <c r="G123">
+        <v>0.9786467855502998</v>
+      </c>
+      <c r="H123">
+        <v>-0.1880002606029876</v>
+      </c>
+      <c r="I123">
+        <v>0.2063576574958056</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>final</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>percentwhite</t>
+        </is>
+      </c>
+      <c r="C124">
+        <v>-0.2065548032647356</v>
+      </c>
+      <c r="D124">
+        <v>0.1827870335999905</v>
+      </c>
+      <c r="E124">
+        <v>315.4356638100126</v>
+      </c>
+      <c r="F124">
+        <v>-1.130029845096991</v>
+      </c>
+      <c r="G124">
+        <v>0.2593221860764572</v>
+      </c>
+      <c r="H124">
+        <v>-0.5803615380229921</v>
+      </c>
+      <c r="I124">
+        <v>0.1443665429860085</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>final</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>percentfreereducedlunch</t>
+        </is>
+      </c>
+      <c r="C125">
+        <v>-0.2842826585855172</v>
+      </c>
+      <c r="D125">
+        <v>0.1580596897268107</v>
+      </c>
+      <c r="E125">
+        <v>317.0402237260061</v>
+      </c>
+      <c r="F125">
+        <v>-1.798577860534014</v>
+      </c>
+      <c r="G125">
+        <v>0.07303654655962386</v>
+      </c>
+      <c r="H125">
+        <v>-0.585810269571882</v>
+      </c>
+      <c r="I125">
+        <v>0.03063556708907537</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>final</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>rplthemes</t>
+        </is>
+      </c>
+      <c r="C126">
+        <v>0.02560258974440326</v>
+      </c>
+      <c r="D126">
+        <v>0.1182957467906876</v>
+      </c>
+      <c r="E126">
+        <v>316.637997772342</v>
+      </c>
+      <c r="F126">
+        <v>0.2164286581638854</v>
+      </c>
+      <c r="G126">
+        <v>0.8287929976275885</v>
+      </c>
+      <c r="H126">
+        <v>-0.1954587710963527</v>
+      </c>
+      <c r="I126">
+        <v>0.2805153924445259</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>final</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>percentblackorafricanamerican</t>
+        </is>
+      </c>
+      <c r="C127">
+        <v>-0.07279015690436529</v>
+      </c>
+      <c r="D127">
+        <v>0.128840786024105</v>
+      </c>
+      <c r="E127">
+        <v>297.659872629958</v>
+      </c>
+      <c r="F127">
+        <v>-0.5649620679180493</v>
+      </c>
+      <c r="G127">
+        <v>0.5725250981915195</v>
+      </c>
+      <c r="H127">
+        <v>-0.3564579871160112</v>
+      </c>
+      <c r="I127">
+        <v>0.1816934877448107</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>final</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>schoollevelHS</t>
+        </is>
+      </c>
+      <c r="C128">
+        <v>0.2676501974802603</v>
+      </c>
+      <c r="D128">
+        <v>0.2389700556321904</v>
+      </c>
+      <c r="E128">
+        <v>313.650595215813</v>
+      </c>
+      <c r="F128">
+        <v>1.120015630293917</v>
+      </c>
+      <c r="G128">
+        <v>0.26356400268227</v>
+      </c>
+      <c r="H128">
+        <v>-0.2051302036231795</v>
+      </c>
+      <c r="I128">
+        <v>0.740804682380788</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>final</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>schoollevelMS</t>
+        </is>
+      </c>
+      <c r="C129">
+        <v>0.2432566602655176</v>
+      </c>
+      <c r="D129">
+        <v>0.2298600700669864</v>
+      </c>
+      <c r="E129">
+        <v>306.1186317208816</v>
+      </c>
+      <c r="F129">
+        <v>1.05828150228366</v>
+      </c>
+      <c r="G129">
+        <v>0.2907614875036456</v>
+      </c>
+      <c r="H129">
+        <v>-0.1898617599644064</v>
+      </c>
+      <c r="I129">
+        <v>0.7106869668769419</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>final</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>cntycaseschange</t>
+        </is>
+      </c>
+      <c r="C130">
+        <v>-0.09897154569938366</v>
+      </c>
+      <c r="D130">
+        <v>0.1658605815490775</v>
+      </c>
+      <c r="E130">
+        <v>51.23465557384009</v>
+      </c>
+      <c r="F130">
+        <v>-0.5967152941043944</v>
+      </c>
+      <c r="G130">
+        <v>0.5533252276744891</v>
+      </c>
+      <c r="H130">
+        <v>-0.461906496659212</v>
+      </c>
+      <c r="I130">
+        <v>0.2809879813586004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>